<commit_message>
new gas dome script and finally fixing DG
</commit_message>
<xml_diff>
--- a/04_Output/rC_DG.xlsx
+++ b/04_Output/rC_DG.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t xml:space="preserve">day</t>
+    <t xml:space="preserve">date</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -447,8 +447,8 @@
       <c r="D2" t="n">
         <v>0.13596180717365</v>
       </c>
-      <c r="E2" t="e">
-        <v>#NUM!</v>
+      <c r="E2" t="n">
+        <v>0.96009522655409</v>
       </c>
       <c r="F2" t="n">
         <v>6744.45857142857</v>
@@ -470,8 +470,8 @@
       <c r="D3" t="n">
         <v>0.399047598709821</v>
       </c>
-      <c r="E3" t="e">
-        <v>#NUM!</v>
+      <c r="E3" t="n">
+        <v>2.15542943540432</v>
       </c>
       <c r="F3" t="n">
         <v>2949.00214285714</v>
@@ -488,19 +488,19 @@
         <v>7</v>
       </c>
       <c r="C4" t="n">
-        <v>442.961367598926</v>
+        <v>519.836014016264</v>
       </c>
       <c r="D4" t="n">
-        <v>0.179033277012746</v>
+        <v>0.292536199651649</v>
       </c>
       <c r="E4" t="n">
-        <v>2.11398960347163</v>
+        <v>1.69234839560588</v>
       </c>
       <c r="F4" t="n">
-        <v>4515.06642857143</v>
+        <v>3847.36714285714</v>
       </c>
       <c r="G4" t="n">
-        <v>857450.978571427</v>
+        <v>447159.985714286</v>
       </c>
     </row>
     <row r="5">
@@ -517,7 +517,7 @@
         <v>0.0872003372604311</v>
       </c>
       <c r="E5" t="n">
-        <v>1.0551824124671</v>
+        <v>1.07758722290172</v>
       </c>
       <c r="F5" t="n">
         <v>17274.5014285714</v>
@@ -528,227 +528,204 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44665</v>
+        <v>44733</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>20.8538613531028</v>
+        <v>2.87311845116259</v>
       </c>
       <c r="D6" t="n">
-        <v>0.160062138915729</v>
+        <v>0.0406457351860475</v>
       </c>
       <c r="E6" t="n">
-        <v>1.29095314351468</v>
+        <v>1.22703041951538</v>
       </c>
       <c r="F6" t="n">
-        <v>4795.275</v>
+        <v>34805.3871428571</v>
       </c>
       <c r="G6" t="n">
-        <v>698040.825</v>
+        <v>15413596.6714286</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44733</v>
+        <v>44817</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>2.87311845116259</v>
+        <v>288.324133991433</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0406457351860475</v>
+        <v>0.194918677610752</v>
       </c>
       <c r="E7" t="n">
-        <v>1.22720288671638</v>
+        <v>1.49757641515283</v>
       </c>
       <c r="F7" t="n">
-        <v>34805.3871428571</v>
+        <v>2774.655</v>
       </c>
       <c r="G7" t="n">
-        <v>15413596.6714286</v>
+        <v>538080.6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44817</v>
+        <v>44879</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>288.324133991433</v>
+        <v>11.2151018074899</v>
       </c>
       <c r="D8" t="n">
-        <v>0.194918677610752</v>
+        <v>0.0351128684887311</v>
       </c>
       <c r="E8" t="n">
-        <v>1.49609686673919</v>
+        <v>1.26005605374847</v>
       </c>
       <c r="F8" t="n">
-        <v>2774.655</v>
+        <v>22291.3714285714</v>
       </c>
       <c r="G8" t="n">
-        <v>538080.6</v>
+        <v>12696981.1285714</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44879</v>
+        <v>44959</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>11.2151018074899</v>
+        <v>2.98137175043788</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0351128684887311</v>
+        <v>0.0129171130222743</v>
       </c>
       <c r="E9" t="n">
-        <v>0.851335002013438</v>
+        <v>1.24406283994386</v>
       </c>
       <c r="F9" t="n">
-        <v>22291.3714285714</v>
+        <v>16770.8035714286</v>
       </c>
       <c r="G9" t="n">
-        <v>12696981.1285714</v>
+        <v>28563478.3821429</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>44959</v>
+        <v>44999</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>2.68544359519209</v>
+        <v>30.839871018848</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0123437852669211</v>
+        <v>0.115971738074685</v>
       </c>
       <c r="E10" t="n">
-        <v>0.829098720167137</v>
+        <v>1.32284879297031</v>
       </c>
       <c r="F10" t="n">
-        <v>18618.8978571429</v>
+        <v>4863.83357142857</v>
       </c>
       <c r="G10" t="n">
-        <v>33183966.1821429</v>
+        <v>1425953.80714286</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>44999</v>
+        <v>45078</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="n">
-        <v>30.839871018848</v>
+        <v>5.46253380723155</v>
       </c>
       <c r="D11" t="n">
-        <v>0.115971738074685</v>
+        <v>0.0391666376832519</v>
       </c>
       <c r="E11" t="n">
-        <v>0.90289706852141</v>
+        <v>1.24855432619956</v>
       </c>
       <c r="F11" t="n">
-        <v>4863.83357142857</v>
+        <v>9153.26142857143</v>
       </c>
       <c r="G11" t="n">
-        <v>1425953.80714286</v>
+        <v>3739207.43571429</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45078</v>
+        <v>45197</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" t="n">
-        <v>48.3070784362028</v>
-      </c>
-      <c r="D12" t="n">
-        <v>-0.00119231592920607</v>
-      </c>
+      <c r="C12"/>
+      <c r="D12"/>
       <c r="E12" t="n">
-        <v>0.832889616253541</v>
+        <v>1.21603948844261</v>
       </c>
       <c r="F12" t="n">
-        <v>1035.04500000001</v>
+        <v>82252.1078571429</v>
       </c>
       <c r="G12" t="n">
-        <v>-13889540.175</v>
+        <v>58777993.6071429</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45197</v>
+        <v>45198</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="C13"/>
-      <c r="D13"/>
+      <c r="C13" t="n">
+        <v>2.03832511291375</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0366654380801947</v>
+      </c>
       <c r="E13" t="n">
-        <v>0.804143083134651</v>
+        <v>1.21047356821986</v>
       </c>
       <c r="F13" t="n">
-        <v>82252.1078571429</v>
+        <v>24529.9435714286</v>
       </c>
       <c r="G13" t="n">
-        <v>58777993.6071429</v>
+        <v>16725521.9464286</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45198</v>
+        <v>45279</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="n">
-        <v>2.03832511291375</v>
+        <v>320.614113433273</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0366654380801947</v>
+        <v>0.274291524526629</v>
       </c>
       <c r="E14" t="n">
-        <v>0.798709265448834</v>
+        <v>1.70055636656728</v>
       </c>
       <c r="F14" t="n">
-        <v>24529.9435714286</v>
+        <v>1871.40857142857</v>
       </c>
       <c r="G14" t="n">
-        <v>16725521.9464286</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>45279</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="n">
-        <v>320.614113433273</v>
-      </c>
-      <c r="D15" t="n">
-        <v>0.274291524526629</v>
-      </c>
-      <c r="E15" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F15" t="n">
-        <v>1871.40857142857</v>
-      </c>
-      <c r="G15" t="n">
         <v>156922.082142857</v>
       </c>
     </row>
@@ -803,7 +780,7 @@
         <v>-0.415059873828465</v>
       </c>
       <c r="E2" t="n">
-        <v>0.805120661779785</v>
+        <v>0.561989668524792</v>
       </c>
       <c r="F2" t="n">
         <v>2055.11785714286</v>
@@ -820,19 +797,19 @@
         <v>16</v>
       </c>
       <c r="C3" t="n">
-        <v>-1522.72807611465</v>
+        <v>1450.59080491212</v>
       </c>
       <c r="D3" t="n">
-        <v>0.574939578921141</v>
-      </c>
-      <c r="E3" t="e">
-        <v>#NUM!</v>
+        <v>0.581036633340369</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.49479210231148</v>
       </c>
       <c r="F3" t="n">
-        <v>-1313.43214285714</v>
+        <v>1378.74857142857</v>
       </c>
       <c r="G3" t="n">
-        <v>-73103.0357142857</v>
+        <v>75933.1714285714</v>
       </c>
     </row>
     <row r="4">
@@ -849,7 +826,7 @@
         <v>0.166262713408938</v>
       </c>
       <c r="E4" t="n">
-        <v>0.586108897296258</v>
+        <v>0.610911641368737</v>
       </c>
       <c r="F4" t="n">
         <v>4953.66642857143</v>
@@ -872,7 +849,7 @@
         <v>0.0375554805809119</v>
       </c>
       <c r="E5" t="n">
-        <v>0.517084102072244</v>
+        <v>0.515695068359833</v>
       </c>
       <c r="F5" t="n">
         <v>29225.04</v>
@@ -895,7 +872,7 @@
         <v>0.426859527793496</v>
       </c>
       <c r="E6" t="n">
-        <v>0.702648046432457</v>
+        <v>0.700626877617393</v>
       </c>
       <c r="F6" t="n">
         <v>2600.08928571429</v>
@@ -918,7 +895,7 @@
         <v>0.131401183260687</v>
       </c>
       <c r="E7" t="n">
-        <v>0.436553212702385</v>
+        <v>0.56429705950321</v>
       </c>
       <c r="F7" t="n">
         <v>20644.0714285714</v>
@@ -941,7 +918,7 @@
         <v>0.0192449199286524</v>
       </c>
       <c r="E8" t="n">
-        <v>0.351646287648636</v>
+        <v>0.517092419639386</v>
       </c>
       <c r="F8" t="n">
         <v>63472.4142857143</v>
@@ -964,7 +941,7 @@
         <v>0.0323205086994282</v>
       </c>
       <c r="E9" t="n">
-        <v>0.465836454475939</v>
+        <v>0.636336976310317</v>
       </c>
       <c r="F9" t="n">
         <v>11464.035</v>
@@ -987,7 +964,7 @@
         <v>0.20143331114612</v>
       </c>
       <c r="E10" t="n">
-        <v>0.338975335223398</v>
+        <v>0.588075516151033</v>
       </c>
       <c r="F10" t="n">
         <v>1878.47571428571</v>
@@ -1009,8 +986,8 @@
       <c r="D11" t="n">
         <v>0.138009949764872</v>
       </c>
-      <c r="E11" t="e">
-        <v>#NUM!</v>
+      <c r="E11" t="n">
+        <v>0.814305514065574</v>
       </c>
       <c r="F11" t="n">
         <v>2495.43</v>
@@ -1058,207 +1035,140 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44292</v>
+        <v>44452</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="n">
-        <v>45.7971257985546</v>
+        <v>7.31312382905134</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0462709643091429</v>
+        <v>0.0186472739593504</v>
       </c>
       <c r="E2" t="n">
-        <v>1.20979881664309</v>
+        <v>1.09512941116791</v>
       </c>
       <c r="F2" t="n">
-        <v>5458.85785714287</v>
+        <v>13674.0471428571</v>
       </c>
       <c r="G2" t="n">
-        <v>3562871.65714287</v>
+        <v>7186340.60357143</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44452</v>
+        <v>44517</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>7.31312382905134</v>
+        <v>22.5234747698149</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0186472739593504</v>
+        <v>0.026820127000421</v>
       </c>
       <c r="E3" t="n">
-        <v>1.07790324035194</v>
+        <v>1.15214486610791</v>
       </c>
       <c r="F3" t="n">
-        <v>13674.0471428571</v>
+        <v>11099.5307142857</v>
       </c>
       <c r="G3" t="n">
-        <v>7186340.60357143</v>
+        <v>11091201.1392857</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44517</v>
+        <v>44589</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>22.5234747698149</v>
+        <v>13.3793659977175</v>
       </c>
       <c r="D4" t="n">
-        <v>0.026820127000421</v>
+        <v>0.0205672011357402</v>
       </c>
       <c r="E4" t="n">
-        <v>1.14604906793147</v>
+        <v>1.18605118392055</v>
       </c>
       <c r="F4" t="n">
-        <v>11099.5307142857</v>
+        <v>3737.09785714286</v>
       </c>
       <c r="G4" t="n">
-        <v>11091201.1392857</v>
+        <v>1835188.37142857</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44589</v>
+        <v>44818</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>13.3793659977175</v>
+        <v>80.2971338081475</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0205672011357402</v>
+        <v>0.0756138674831853</v>
       </c>
       <c r="E5" t="n">
-        <v>1.15697656532308</v>
+        <v>1.33613727954729</v>
       </c>
       <c r="F5" t="n">
-        <v>3737.09785714286</v>
+        <v>4981.49785714286</v>
       </c>
       <c r="G5" t="n">
-        <v>1835188.37142857</v>
+        <v>1686547.05</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44666</v>
+        <v>44998</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>8.55028667889765</v>
+        <v>73.3277604235412</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0127442482204935</v>
+        <v>0.0601797177022106</v>
       </c>
       <c r="E6" t="n">
-        <v>1.13564203007194</v>
+        <v>1.28317296907321</v>
       </c>
       <c r="F6" t="n">
-        <v>17543.2714285714</v>
+        <v>6818.7</v>
       </c>
       <c r="G6" t="n">
-        <v>11838449.1321429</v>
+        <v>2266112.325</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44818</v>
+        <v>45140</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>80.2971338081475</v>
+        <v>203.61423579318</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0756138674831853</v>
+        <v>0.151213418262108</v>
       </c>
       <c r="E7" t="n">
-        <v>1.35380599386199</v>
+        <v>1.47757506242285</v>
       </c>
       <c r="F7" t="n">
-        <v>4981.49785714286</v>
+        <v>6875.74714285714</v>
       </c>
       <c r="G7" t="n">
-        <v>1686547.05</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>44998</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="n">
-        <v>73.3277604235412</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.0601797177022106</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1.24278759368125</v>
-      </c>
-      <c r="F8" t="n">
-        <v>6818.7</v>
-      </c>
-      <c r="G8" t="n">
-        <v>2266112.325</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>45140</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="n">
-        <v>203.61423579318</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.151213418262108</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1.50181571590416</v>
-      </c>
-      <c r="F9" t="n">
-        <v>6875.74714285714</v>
-      </c>
-      <c r="G9" t="n">
         <v>682057.242857143</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>45279</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="n">
-        <v>587.941323455919</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.116204075358259</v>
-      </c>
-      <c r="E10"/>
-      <c r="F10" t="n">
-        <v>2041.02</v>
-      </c>
-      <c r="G10" t="n">
-        <v>298589.7</v>
       </c>
     </row>
   </sheetData>
@@ -1306,19 +1216,19 @@
         <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>191.781610061411</v>
+        <v>218.653058116812</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0247622262125784</v>
+        <v>0.0308372725815327</v>
       </c>
       <c r="E2" t="n">
-        <v>1.05344544680825</v>
+        <v>1.11553844289507</v>
       </c>
       <c r="F2" t="n">
-        <v>6257.11714285714</v>
+        <v>5488.14642857143</v>
       </c>
       <c r="G2" t="n">
-        <v>6923650.89642856</v>
+        <v>4876410.9</v>
       </c>
     </row>
     <row r="3">
@@ -1335,7 +1245,7 @@
         <v>0.028469917352607</v>
       </c>
       <c r="E3" t="n">
-        <v>0.79805472226329</v>
+        <v>0.813657725497269</v>
       </c>
       <c r="F3" t="n">
         <v>24196.695</v>
@@ -1358,7 +1268,7 @@
         <v>0.230530622192957</v>
       </c>
       <c r="E4" t="n">
-        <v>0.929157175246169</v>
+        <v>0.925645449472718</v>
       </c>
       <c r="F4" t="n">
         <v>7971.19071428572</v>
@@ -1381,7 +1291,7 @@
         <v>0.0173910258844274</v>
       </c>
       <c r="E5" t="n">
-        <v>0.832412029104361</v>
+        <v>0.857244517216307</v>
       </c>
       <c r="F5" t="n">
         <v>11892.435</v>
@@ -1392,116 +1302,93 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44659</v>
+        <v>44733</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>37.7739793942942</v>
+        <v>5.84854833181856</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0147219520870121</v>
+        <v>0.0217811972641943</v>
       </c>
       <c r="E6" t="n">
-        <v>0.948484510302354</v>
+        <v>0.838387320411005</v>
       </c>
       <c r="F6" t="n">
-        <v>7941.975</v>
+        <v>8549.13</v>
       </c>
       <c r="G6" t="n">
-        <v>7714346.7</v>
+        <v>3925004.625</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44733</v>
+        <v>44806</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>5.84854833181856</v>
+        <v>94.0961393698247</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0217811972641943</v>
+        <v>0.125964440018116</v>
       </c>
       <c r="E7" t="n">
-        <v>0.838920867879614</v>
+        <v>1.03416328014474</v>
       </c>
       <c r="F7" t="n">
-        <v>8549.13</v>
+        <v>6376.45714285715</v>
       </c>
       <c r="G7" t="n">
-        <v>3925004.625</v>
+        <v>1543943.21785715</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44806</v>
+        <v>44998</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="n">
-        <v>94.0961393698247</v>
+        <v>4.110400422878</v>
       </c>
       <c r="D8" t="n">
-        <v>0.125964440018116</v>
+        <v>0.0135347353218176</v>
       </c>
       <c r="E8" t="n">
-        <v>1.0467996217053</v>
+        <v>0.852390189325833</v>
       </c>
       <c r="F8" t="n">
-        <v>6376.45714285715</v>
+        <v>121642.65</v>
       </c>
       <c r="G8" t="n">
-        <v>1543943.21785715</v>
+        <v>139305352.5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44998</v>
+        <v>45279</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>4.110400422878</v>
+        <v>850.231688135016</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0135347353218176</v>
+        <v>-0.264707017120813</v>
       </c>
       <c r="E9" t="n">
-        <v>0.806710352094947</v>
+        <v>1.23215856249894</v>
       </c>
       <c r="F9" t="n">
-        <v>121642.65</v>
+        <v>1999.455</v>
       </c>
       <c r="G9" t="n">
-        <v>139305352.5</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>45279</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="n">
-        <v>850.231688135016</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-0.264707017120813</v>
-      </c>
-      <c r="E10" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1999.455</v>
-      </c>
-      <c r="G10" t="n">
         <v>-105748.499999999</v>
       </c>
     </row>
@@ -1550,19 +1437,19 @@
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>190.28163721039</v>
+        <v>201.556447682785</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0860186407696766</v>
+        <v>0.0966260418499097</v>
       </c>
       <c r="E2" t="n">
-        <v>0.984838957026399</v>
+        <v>0.947540539626533</v>
       </c>
       <c r="F2" t="n">
-        <v>2102.14714285714</v>
+        <v>1984.55571428571</v>
       </c>
       <c r="G2" t="n">
-        <v>745367.36785714</v>
+        <v>626424.803571428</v>
       </c>
     </row>
     <row r="3">
@@ -1579,7 +1466,7 @@
         <v>0.0482196240014123</v>
       </c>
       <c r="E3" t="n">
-        <v>0.956786249405832</v>
+        <v>0.954603621934516</v>
       </c>
       <c r="F3" t="n">
         <v>14294.7535714286</v>
@@ -1602,7 +1489,7 @@
         <v>0.0396467471682954</v>
       </c>
       <c r="E4" t="n">
-        <v>0.992405077407557</v>
+        <v>0.994357678715358</v>
       </c>
       <c r="F4" t="n">
         <v>9733.09499999999</v>
@@ -1625,7 +1512,7 @@
         <v>0.0240540549037401</v>
       </c>
       <c r="E5" t="n">
-        <v>0.915689097744538</v>
+        <v>0.925241631392354</v>
       </c>
       <c r="F5" t="n">
         <v>5443.77642857143</v>
@@ -1636,47 +1523,24 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44666</v>
+        <v>44818</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>43.1380098171326</v>
+        <v>268.141444612033</v>
       </c>
       <c r="D6" t="n">
-        <v>0.026222037675287</v>
+        <v>0.117343468865951</v>
       </c>
       <c r="E6" t="n">
-        <v>0.917982841622249</v>
+        <v>1.29046111183131</v>
       </c>
       <c r="F6" t="n">
-        <v>9272.565</v>
+        <v>2237.625</v>
       </c>
       <c r="G6" t="n">
-        <v>14109328.5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>44818</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="n">
-        <v>268.141444612033</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.117343468865951</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1.29257475242223</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2237.625</v>
-      </c>
-      <c r="G7" t="n">
         <v>444308.174999999</v>
       </c>
     </row>
@@ -1730,8 +1594,8 @@
       <c r="D2" t="n">
         <v>0.387436294953374</v>
       </c>
-      <c r="E2" t="e">
-        <v>#NUM!</v>
+      <c r="E2" t="n">
+        <v>1.72322186462555</v>
       </c>
       <c r="F2" t="n">
         <v>1203.56357142857</v>
@@ -1754,7 +1618,7 @@
         <v>0.0748083206536477</v>
       </c>
       <c r="E3" t="n">
-        <v>0.877273800351796</v>
+        <v>0.929733787750404</v>
       </c>
       <c r="F3" t="n">
         <v>11714.8821428571</v>
@@ -1777,7 +1641,7 @@
         <v>0.181034619271933</v>
       </c>
       <c r="E4" t="n">
-        <v>1.16981620446827</v>
+        <v>1.16430483770059</v>
       </c>
       <c r="F4" t="n">
         <v>4287.97071428572</v>
@@ -1800,7 +1664,7 @@
         <v>0.0466003004043193</v>
       </c>
       <c r="E5" t="n">
-        <v>0.937617911788854</v>
+        <v>0.95598794379407</v>
       </c>
       <c r="F5" t="n">
         <v>3619.28785714286</v>
@@ -1823,7 +1687,7 @@
         <v>0.0247248402753767</v>
       </c>
       <c r="E6" t="n">
-        <v>0.874297936664055</v>
+        <v>0.878364493092622</v>
       </c>
       <c r="F6" t="n">
         <v>20718.7864285714</v>
@@ -1840,87 +1704,64 @@
         <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>83.1668955835468</v>
+        <v>83.4160791046595</v>
       </c>
       <c r="D7" t="n">
-        <v>0.103420283876735</v>
+        <v>0.104270024651914</v>
       </c>
       <c r="E7" t="n">
-        <v>1.16006263382476</v>
+        <v>1.12718696043453</v>
       </c>
       <c r="F7" t="n">
-        <v>12024.015</v>
+        <v>11988.0964285714</v>
       </c>
       <c r="G7" t="n">
-        <v>4290127.01249999</v>
+        <v>4242453.76071428</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44879</v>
+        <v>44959</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>62.1041048151678</v>
+        <v>30.1205661719794</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0624314324451668</v>
+        <v>0.017179789481342</v>
       </c>
       <c r="E8" t="n">
-        <v>0.822189599549654</v>
+        <v>0.994350520519222</v>
       </c>
       <c r="F8" t="n">
-        <v>7245.89785714286</v>
+        <v>6639.98142857143</v>
       </c>
       <c r="G8" t="n">
-        <v>3017604.06428571</v>
+        <v>10435488.675</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44959</v>
+        <v>44999</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="n">
-        <v>27.7456390791777</v>
+        <v>203.383280877396</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0274136731817164</v>
+        <v>0.223866557705922</v>
       </c>
       <c r="E9" t="n">
-        <v>0.971485525319535</v>
+        <v>1.16293097131649</v>
       </c>
       <c r="F9" t="n">
-        <v>7208.34</v>
+        <v>2950.095</v>
       </c>
       <c r="G9" t="n">
-        <v>7099565.925</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>44999</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="n">
-        <v>203.383280877396</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.223866557705922</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1.16201921604601</v>
-      </c>
-      <c r="F10" t="n">
-        <v>2950.095</v>
-      </c>
-      <c r="G10" t="n">
         <v>466498.274999997</v>
       </c>
     </row>
@@ -1975,7 +1816,7 @@
         <v>0.0288993102026876</v>
       </c>
       <c r="E2" t="n">
-        <v>0.986430878316302</v>
+        <v>0.235947559167846</v>
       </c>
       <c r="F2" t="n">
         <v>4290.66642857143</v>
@@ -1997,8 +1838,8 @@
       <c r="D3" t="n">
         <v>0.233297132170326</v>
       </c>
-      <c r="E3" t="e">
-        <v>#NUM!</v>
+      <c r="E3" t="n">
+        <v>3.00425309577892</v>
       </c>
       <c r="F3" t="n">
         <v>3691.38</v>
@@ -2020,8 +1861,8 @@
       <c r="D4" t="n">
         <v>0.0334046106509795</v>
       </c>
-      <c r="E4" t="e">
-        <v>#NUM!</v>
+      <c r="E4" t="n">
+        <v>1.11679553298501</v>
       </c>
       <c r="F4" t="n">
         <v>24413.1324193548</v>
@@ -2032,93 +1873,70 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44510</v>
+        <v>44659</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>21.1919407049499</v>
+        <v>10.1562152863735</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0277510769684758</v>
+        <v>0.0160991553702436</v>
       </c>
       <c r="E5" t="n">
-        <v>1.14205940927033</v>
+        <v>1.20205744593307</v>
       </c>
       <c r="F5" t="n">
-        <v>9437.55</v>
+        <v>19692.375</v>
       </c>
       <c r="G5" t="n">
-        <v>5271219.75</v>
+        <v>12231930.525</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44659</v>
+        <v>44806</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>10.1562152863735</v>
+        <v>35.2877784497159</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0160991553702436</v>
+        <v>0.0598939505762173</v>
       </c>
       <c r="E6" t="n">
-        <v>1.19490494036932</v>
+        <v>1.21757509060473</v>
       </c>
       <c r="F6" t="n">
-        <v>19692.375</v>
+        <v>22670.7385714286</v>
       </c>
       <c r="G6" t="n">
-        <v>12231930.525</v>
+        <v>9576420.99642858</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44806</v>
+        <v>45197</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>35.2877784497159</v>
+        <v>18.5478970626159</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0598939505762173</v>
+        <v>0.0380123901994629</v>
       </c>
       <c r="E7" t="n">
-        <v>1.21849834055729</v>
+        <v>1.19617447962169</v>
       </c>
       <c r="F7" t="n">
-        <v>22670.7385714286</v>
+        <v>10782.8935714286</v>
       </c>
       <c r="G7" t="n">
-        <v>9576420.99642858</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>45197</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="n">
-        <v>18.5478970626159</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.0380123901994629</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1.28420761962736</v>
-      </c>
-      <c r="F8" t="n">
-        <v>10782.8935714286</v>
-      </c>
-      <c r="G8" t="n">
         <v>5673357.30000001</v>
       </c>
     </row>
@@ -2167,19 +1985,19 @@
         <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>1506.92945363582</v>
+        <v>1474.27392009435</v>
       </c>
       <c r="D2" t="n">
-        <v>0.638751845267524</v>
+        <v>0.609595398242257</v>
       </c>
       <c r="E2" t="n">
-        <v>0.953145766518806</v>
+        <v>0.588459099645472</v>
       </c>
       <c r="F2" t="n">
-        <v>1327.20214285714</v>
+        <v>1356.6</v>
       </c>
       <c r="G2" t="n">
-        <v>103890.278571429</v>
+        <v>111270.525</v>
       </c>
     </row>
     <row r="3">
@@ -2196,7 +2014,7 @@
         <v>0.19909322659857</v>
       </c>
       <c r="E3" t="n">
-        <v>1.0572381622036</v>
+        <v>1.05548560188029</v>
       </c>
       <c r="F3" t="n">
         <v>6115.665</v>
@@ -2219,7 +2037,7 @@
         <v>0.09276270132275</v>
       </c>
       <c r="E4" t="n">
-        <v>0.981083073137467</v>
+        <v>1.01102869478466</v>
       </c>
       <c r="F4" t="n">
         <v>7616.01214285714</v>
@@ -2236,19 +2054,19 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>32.9631299151117</v>
+        <v>33.6536236839781</v>
       </c>
       <c r="D5" t="n">
-        <v>0.130442083405527</v>
+        <v>0.132219643097552</v>
       </c>
       <c r="E5" t="n">
-        <v>1.08686776782644</v>
+        <v>0.907178487084247</v>
       </c>
       <c r="F5" t="n">
-        <v>18202.155</v>
+        <v>17828.6892857143</v>
       </c>
       <c r="G5" t="n">
-        <v>3767635.2</v>
+        <v>3640719.33214286</v>
       </c>
     </row>
     <row r="6">
@@ -2264,8 +2082,8 @@
       <c r="D6" t="n">
         <v>0.370207050897618</v>
       </c>
-      <c r="E6" t="e">
-        <v>#NUM!</v>
+      <c r="E6" t="n">
+        <v>1.43410908639999</v>
       </c>
       <c r="F6" t="n">
         <v>1394.12142857143</v>
@@ -2288,7 +2106,7 @@
         <v>0.108285591446864</v>
       </c>
       <c r="E7" t="n">
-        <v>1.02273348879362</v>
+        <v>0.684173748145478</v>
       </c>
       <c r="F7" t="n">
         <v>9619.32857142857</v>
@@ -2311,7 +2129,7 @@
         <v>0.0176083819768147</v>
       </c>
       <c r="E8" t="n">
-        <v>1.3112326247001</v>
+        <v>1.13760053883744</v>
       </c>
       <c r="F8" t="n">
         <v>19459.2321428571</v>
@@ -2334,7 +2152,7 @@
         <v>0.0942639400766061</v>
       </c>
       <c r="E9" t="n">
-        <v>1.40222411823612</v>
+        <v>1.2351274384367</v>
       </c>
       <c r="F9" t="n">
         <v>18083.6892857143</v>
@@ -2357,7 +2175,7 @@
         <v>-0.624858780565361</v>
       </c>
       <c r="E10" t="n">
-        <v>1.85235323819132</v>
+        <v>1.70007552742378</v>
       </c>
       <c r="F10" t="n">
         <v>1823.90571428572</v>
@@ -2380,7 +2198,7 @@
         <v>0.0966021881464723</v>
       </c>
       <c r="E11" t="n">
-        <v>1.55357252699354</v>
+        <v>1.38542489812252</v>
       </c>
       <c r="F11" t="n">
         <v>750.027857142865</v>
@@ -2403,7 +2221,7 @@
         <v>0.0456410932698102</v>
       </c>
       <c r="E12" t="n">
-        <v>1.53012743843669</v>
+        <v>1.2714292155857</v>
       </c>
       <c r="F12" t="n">
         <v>2880.99</v>
@@ -2425,8 +2243,8 @@
       <c r="D13" t="n">
         <v>0.229962718506469</v>
       </c>
-      <c r="E13" t="e">
-        <v>#NUM!</v>
+      <c r="E13" t="n">
+        <v>1.46778642648194</v>
       </c>
       <c r="F13" t="n">
         <v>2535.975</v>
@@ -2486,7 +2304,7 @@
         <v>0.0836415522456026</v>
       </c>
       <c r="E2" t="n">
-        <v>0.955689483651695</v>
+        <v>0.391831821845463</v>
       </c>
       <c r="F2" t="n">
         <v>2500.85785714285</v>
@@ -2509,7 +2327,7 @@
         <v>0.10472695502504</v>
       </c>
       <c r="E3" t="n">
-        <v>1.00749398277837</v>
+        <v>0.999480006838803</v>
       </c>
       <c r="F3" t="n">
         <v>13985.22</v>
@@ -2520,117 +2338,71 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44517</v>
+        <v>44589</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>18.4922954162685</v>
+        <v>6.79493167987407</v>
       </c>
       <c r="D4" t="n">
-        <v>0.068927815528573</v>
+        <v>0.0279077813421051</v>
       </c>
       <c r="E4" t="n">
-        <v>1.03909095253797</v>
+        <v>1.01485820994369</v>
       </c>
       <c r="F4" t="n">
-        <v>10815.315</v>
+        <v>14716.8514285714</v>
       </c>
       <c r="G4" t="n">
-        <v>3342137.1</v>
+        <v>4798781.61428571</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44589</v>
+        <v>44818</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>-1084.1619428182</v>
+        <v>52.7801968701343</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0419823989213417</v>
+        <v>0.0490018181170012</v>
       </c>
       <c r="E5" t="n">
-        <v>0.992939568297968</v>
+        <v>1.15128049983373</v>
       </c>
       <c r="F5" t="n">
-        <v>-92.2371428571427</v>
+        <v>7578.6</v>
       </c>
       <c r="G5" t="n">
-        <v>-19993.0928571428</v>
+        <v>3433442.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44665</v>
+        <v>45279</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>5.55093440266534</v>
+        <v>409.296138546743</v>
       </c>
       <c r="D6" t="n">
-        <v>0.143169282902277</v>
+        <v>0.0895346799829791</v>
       </c>
       <c r="E6" t="n">
-        <v>0.986715966159205</v>
+        <v>1.36819286547664</v>
       </c>
       <c r="F6" t="n">
-        <v>18014.985</v>
+        <v>1954.575</v>
       </c>
       <c r="G6" t="n">
-        <v>1535125.5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>44818</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="n">
-        <v>52.7801968701343</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.0490018181170012</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1.11766819484688</v>
-      </c>
-      <c r="F7" t="n">
-        <v>7578.6</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3433442.4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>45279</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="n">
-        <v>409.983838583506</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.0897427663635656</v>
-      </c>
-      <c r="E8" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="F8" t="n">
-        <v>1951.29642857143</v>
-      </c>
-      <c r="G8" t="n">
-        <v>456607.553571429</v>
+        <v>458437.725</v>
       </c>
     </row>
   </sheetData>
@@ -2684,7 +2456,7 @@
         <v>0.0578152666505854</v>
       </c>
       <c r="E2" t="n">
-        <v>0.97482200093188</v>
+        <v>0.871378375484023</v>
       </c>
       <c r="F2" t="n">
         <v>2261.85</v>
@@ -2695,94 +2467,163 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44589</v>
+        <v>44452</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>4.49444319884161</v>
+        <v>19.0713037906123</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0437964783271548</v>
+        <v>0.111120888231963</v>
       </c>
       <c r="E3" t="n">
-        <v>0.817167425950112</v>
+        <v>0.875693725023813</v>
       </c>
       <c r="F3" t="n">
-        <v>11124.8485714286</v>
+        <v>7865.22</v>
       </c>
       <c r="G3" t="n">
-        <v>2159105.4</v>
+        <v>1033398.975</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44666</v>
+        <v>44517</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>2.89214023293876</v>
+        <v>16.9350140609002</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0252018268584692</v>
+        <v>0.0463166323010258</v>
       </c>
       <c r="E4" t="n">
-        <v>0.789406482890101</v>
+        <v>0.861109604946484</v>
       </c>
       <c r="F4" t="n">
-        <v>17288.235</v>
+        <v>11809.8514285714</v>
       </c>
       <c r="G4" t="n">
-        <v>11318857.125</v>
+        <v>10479710.4107143</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44966</v>
+        <v>44589</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="n">
-        <v>8.00184819830957</v>
+        <v>4.49444319884161</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0131382698505472</v>
+        <v>0.0437964783271548</v>
       </c>
       <c r="E5" t="n">
-        <v>0.81136811023622</v>
+        <v>0.829087949994082</v>
       </c>
       <c r="F5" t="n">
-        <v>6248.55642857143</v>
+        <v>11124.8485714286</v>
       </c>
       <c r="G5" t="n">
-        <v>6658394.97857143</v>
+        <v>2159105.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44998</v>
+        <v>44666</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>148.679429308878</v>
+        <v>2.89214023293876</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.15252734905357</v>
+        <v>0.0252018268584692</v>
       </c>
       <c r="E6" t="n">
-        <v>1.02550045137969</v>
+        <v>0.631433198623971</v>
       </c>
       <c r="F6" t="n">
-        <v>3362.94000000001</v>
+        <v>17288.235</v>
       </c>
       <c r="G6" t="n">
-        <v>-81700.7249999963</v>
+        <v>11318857.125</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>44818</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="n">
+        <v>105.628429740967</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.142353917790553</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.04927645855292</v>
+      </c>
+      <c r="F7" t="n">
+        <v>7573.71857142857</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2255825.98928571</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>44966</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>8.00184819830957</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0131382698505472</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.778096370738196</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6248.55642857143</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6658394.97857143</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>44998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="n">
+        <v>126.543034122329</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.154867311917387</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.09144358834172</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3951.225</v>
+      </c>
+      <c r="G9" t="n">
+        <v>714381.225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update scripts and files
</commit_message>
<xml_diff>
--- a/04_Output/rC_DG.xlsx
+++ b/04_Output/rC_DG.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t xml:space="preserve">m_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logQ</t>
   </si>
   <si>
     <t xml:space="preserve">13</t>
@@ -433,13 +436,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44299</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="n">
         <v>14.8269870651483</v>
@@ -448,13 +454,16 @@
         <v>0.13596180717365</v>
       </c>
       <c r="E2" t="n">
-        <v>0.96009522655409</v>
+        <v>-0.236734445416943</v>
       </c>
       <c r="F2" t="n">
         <v>6744.45857142857</v>
       </c>
       <c r="G2" t="n">
         <v>997071.310714285</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.17105290868724</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +471,7 @@
         <v>44386</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
         <v>406.917303504357</v>
@@ -471,13 +480,16 @@
         <v>0.399047598709821</v>
       </c>
       <c r="E3" t="n">
-        <v>2.15542943540432</v>
+        <v>0.571842117623629</v>
       </c>
       <c r="F3" t="n">
         <v>2949.00214285714</v>
       </c>
       <c r="G3" t="n">
         <v>204705.803571429</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.60950615792082</v>
       </c>
     </row>
     <row r="4">
@@ -485,7 +497,7 @@
         <v>44459</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="n">
         <v>519.836014016264</v>
@@ -494,13 +506,16 @@
         <v>0.292536199651649</v>
       </c>
       <c r="E4" t="n">
-        <v>1.69234839560588</v>
+        <v>0.533948504904586</v>
       </c>
       <c r="F4" t="n">
         <v>3847.36714285714</v>
       </c>
       <c r="G4" t="n">
         <v>447159.985714286</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.71586636394285</v>
       </c>
     </row>
     <row r="5">
@@ -508,7 +523,7 @@
         <v>44589</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
         <v>11.5777581672607</v>
@@ -517,7 +532,7 @@
         <v>0.0872003372604311</v>
       </c>
       <c r="E5" t="n">
-        <v>1.07758722290172</v>
+        <v>-0.112291787026756</v>
       </c>
       <c r="F5" t="n">
         <v>17274.5014285714</v>
@@ -525,208 +540,266 @@
       <c r="G5" t="n">
         <v>3328102.08214286</v>
       </c>
+      <c r="H5" t="n">
+        <v>1.06362447391267</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44733</v>
+        <v>44665</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>2.87311845116259</v>
+        <v>20.8538613531028</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0406457351860475</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1.22703041951538</v>
-      </c>
+        <v>0.160062138915729</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="n">
-        <v>34805.3871428571</v>
+        <v>4795.275</v>
       </c>
       <c r="G6" t="n">
-        <v>15413596.6714286</v>
+        <v>698040.825</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.31918648180763</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44817</v>
+        <v>44733</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>288.324133991433</v>
+        <v>2.87311845116259</v>
       </c>
       <c r="D7" t="n">
-        <v>0.194918677610752</v>
+        <v>0.0406457351860475</v>
       </c>
       <c r="E7" t="n">
-        <v>1.49757641515283</v>
+        <v>0.0569027203963497</v>
       </c>
       <c r="F7" t="n">
-        <v>2774.655</v>
+        <v>34805.3871428571</v>
       </c>
       <c r="G7" t="n">
-        <v>538080.6</v>
+        <v>15413596.6714286</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.458353531187161</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44879</v>
+        <v>44817</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" t="n">
-        <v>11.2151018074899</v>
+        <v>288.324133991433</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0351128684887311</v>
+        <v>0.194918677610752</v>
       </c>
       <c r="E8" t="n">
-        <v>1.26005605374847</v>
+        <v>0.326424187469587</v>
       </c>
       <c r="F8" t="n">
-        <v>22291.3714285714</v>
+        <v>2774.655</v>
       </c>
       <c r="G8" t="n">
-        <v>12696981.1285714</v>
+        <v>538080.6</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.45988099625789</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44959</v>
+        <v>44879</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>2.98137175043788</v>
+        <v>11.2151018074899</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0129171130222743</v>
+        <v>0.0351128684887311</v>
       </c>
       <c r="E9" t="n">
-        <v>1.24406283994386</v>
+        <v>0.0913046673568094</v>
       </c>
       <c r="F9" t="n">
-        <v>16770.8035714286</v>
+        <v>22291.3714285714</v>
       </c>
       <c r="G9" t="n">
-        <v>28563478.3821429</v>
+        <v>12696981.1285714</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.0498032203381</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>44999</v>
+        <v>44959</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>30.839871018848</v>
+        <v>2.98137175043788</v>
       </c>
       <c r="D10" t="n">
-        <v>0.115971738074685</v>
+        <v>0.0129171130222743</v>
       </c>
       <c r="E10" t="n">
-        <v>1.32284879297031</v>
+        <v>0.0686781937579025</v>
       </c>
       <c r="F10" t="n">
-        <v>4863.83357142857</v>
+        <v>16770.8035714286</v>
       </c>
       <c r="G10" t="n">
-        <v>1425953.80714286</v>
+        <v>28563478.3821429</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.474416132053351</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45078</v>
+        <v>44999</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>5.46253380723155</v>
+        <v>30.839871018848</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0391666376832519</v>
+        <v>0.115971738074685</v>
       </c>
       <c r="E11" t="n">
-        <v>1.24855432619956</v>
+        <v>0.143757202817436</v>
       </c>
       <c r="F11" t="n">
-        <v>9153.26142857143</v>
+        <v>4863.83357142857</v>
       </c>
       <c r="G11" t="n">
-        <v>3739207.43571429</v>
+        <v>1425953.80714286</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.48911255303911</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45197</v>
+        <v>45078</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12"/>
+        <v>8</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.46253380723155</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0391666376832519</v>
+      </c>
       <c r="E12" t="n">
-        <v>1.21603948844261</v>
+        <v>0.0728896162535407</v>
       </c>
       <c r="F12" t="n">
-        <v>82252.1078571429</v>
+        <v>9153.26142857143</v>
       </c>
       <c r="G12" t="n">
-        <v>58777993.6071429</v>
+        <v>3739207.43571429</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.737394137804323</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45198</v>
+        <v>45142</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>2.03832511291375</v>
+        <v>54.429152876328</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0366654380801947</v>
+        <v>0.145089110762292</v>
       </c>
       <c r="E13" t="n">
-        <v>1.21047356821986</v>
+        <v>0.19325455560002</v>
       </c>
       <c r="F13" t="n">
-        <v>24529.9435714286</v>
+        <v>11023.5042857143</v>
       </c>
       <c r="G13" t="n">
-        <v>16725521.9464286</v>
+        <v>2583234.15</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.73583157510342</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
+        <v>45198</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2.03832511291375</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0366654380801947</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.038709265448834</v>
+      </c>
+      <c r="F14" t="n">
+        <v>24529.9435714286</v>
+      </c>
+      <c r="G14" t="n">
+        <v>16725521.9464286</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.309273455177549</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
         <v>45279</v>
       </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="n">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="n">
         <v>320.614113433273</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D15" t="n">
         <v>0.274291524526629</v>
       </c>
-      <c r="E14" t="n">
-        <v>1.70055636656728</v>
-      </c>
-      <c r="F14" t="n">
+      <c r="E15" t="n">
+        <v>0.535585069806503</v>
+      </c>
+      <c r="F15" t="n">
         <v>1871.40857142857</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G15" t="n">
         <v>156922.082142857</v>
+      </c>
+      <c r="H15" t="n">
+        <v>2.50598263608201</v>
       </c>
     </row>
   </sheetData>
@@ -765,13 +838,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44302</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="n">
         <v>243.295049119533</v>
@@ -780,13 +856,16 @@
         <v>-0.415059873828465</v>
       </c>
       <c r="E2" t="n">
-        <v>0.561989668524792</v>
+        <v>0.144474375522178</v>
       </c>
       <c r="F2" t="n">
         <v>2055.11785714286</v>
       </c>
       <c r="G2" t="n">
         <v>-165871.125</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.38613327143824</v>
       </c>
     </row>
     <row r="3">
@@ -794,22 +873,25 @@
         <v>44386</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>1450.59080491212</v>
+        <v>1444.94054069675</v>
       </c>
       <c r="D3" t="n">
-        <v>0.581036633340369</v>
+        <v>0.577927133588421</v>
       </c>
       <c r="E3" t="n">
-        <v>1.49479210231148</v>
+        <v>0.835018144430228</v>
       </c>
       <c r="F3" t="n">
-        <v>1378.74857142857</v>
+        <v>1384.14</v>
       </c>
       <c r="G3" t="n">
-        <v>75933.1714285714</v>
+        <v>76640.25</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.15984997624233</v>
       </c>
     </row>
     <row r="4">
@@ -817,7 +899,7 @@
         <v>44589</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="n">
         <v>60.5612033684141</v>
@@ -826,7 +908,7 @@
         <v>0.166262713408938</v>
       </c>
       <c r="E4" t="n">
-        <v>0.610911641368737</v>
+        <v>-0.0713653021975958</v>
       </c>
       <c r="F4" t="n">
         <v>4953.66642857143</v>
@@ -834,167 +916,233 @@
       <c r="G4" t="n">
         <v>953414.764285715</v>
       </c>
+      <c r="H4" t="n">
+        <v>1.78219449613319</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44733</v>
+        <v>44665</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>3.42172328934366</v>
+        <v>156.869264340194</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0375554805809119</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.515695068359833</v>
-      </c>
+        <v>0.0999742912566901</v>
+      </c>
+      <c r="E5"/>
       <c r="F5" t="n">
-        <v>29225.04</v>
+        <v>3506.10428571429</v>
       </c>
       <c r="G5" t="n">
-        <v>9727288.65000001</v>
+        <v>1052101.76785714</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2.1955378598709</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44817</v>
+        <v>44733</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="n">
-        <v>173.070979705367</v>
+        <v>3.42172328934366</v>
       </c>
       <c r="D6" t="n">
-        <v>0.426859527793496</v>
+        <v>0.0375554805809119</v>
       </c>
       <c r="E6" t="n">
-        <v>0.700626877617393</v>
+        <v>-0.143216064247785</v>
       </c>
       <c r="F6" t="n">
-        <v>2600.08928571429</v>
+        <v>29225.04</v>
       </c>
       <c r="G6" t="n">
-        <v>200400.675000005</v>
+        <v>9727288.65000001</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.534244885751498</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44879</v>
+        <v>44817</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="n">
-        <v>16.9540200057436</v>
+        <v>173.070979705367</v>
       </c>
       <c r="D7" t="n">
-        <v>0.131401183260687</v>
+        <v>0.426859527793496</v>
       </c>
       <c r="E7" t="n">
-        <v>0.56429705950321</v>
+        <v>0.0429753671628554</v>
       </c>
       <c r="F7" t="n">
-        <v>20644.0714285714</v>
+        <v>2600.08928571429</v>
       </c>
       <c r="G7" t="n">
-        <v>3189276.075</v>
+        <v>200400.675000005</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.23822425210174</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44953</v>
+        <v>44879</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="n">
-        <v>1.57548757401697</v>
+        <v>16.9540200057436</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0192449199286524</v>
+        <v>0.131401183260687</v>
       </c>
       <c r="E8" t="n">
-        <v>0.517092419639386</v>
+        <v>-0.0888937886209107</v>
       </c>
       <c r="F8" t="n">
-        <v>63472.4142857143</v>
+        <v>20644.0714285714</v>
       </c>
       <c r="G8" t="n">
-        <v>64313703.7285714</v>
+        <v>3189276.075</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.22927269128908</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44999</v>
+        <v>44953</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>17.4458643924238</v>
+        <v>1.57548757401697</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0323205086994282</v>
+        <v>0.0192449199286524</v>
       </c>
       <c r="E9" t="n">
-        <v>0.636336976310317</v>
+        <v>0.0323948686912526</v>
       </c>
       <c r="F9" t="n">
-        <v>11464.035</v>
+        <v>63472.4142857143</v>
       </c>
       <c r="G9" t="n">
-        <v>11705049.525</v>
+        <v>64313703.7285714</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.197414982211926</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45231</v>
+        <v>44999</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>26.617325749677</v>
+        <v>17.4458643924238</v>
       </c>
       <c r="D10" t="n">
-        <v>0.20143331114612</v>
+        <v>0.0323205086994282</v>
       </c>
       <c r="E10" t="n">
-        <v>0.588075516151033</v>
+        <v>0.146696588771965</v>
       </c>
       <c r="F10" t="n">
-        <v>1878.47571428571</v>
+        <v>11464.035</v>
       </c>
       <c r="G10" t="n">
-        <v>141748.307142857</v>
+        <v>11705049.525</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.24169249236021</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="n">
+        <v>26.617325749677</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.20143331114612</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.102308668556731</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1878.47571428571</v>
+      </c>
+      <c r="G11" t="n">
+        <v>141748.307142857</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.42516441963977</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
         <v>45296</v>
       </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="n">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="n">
         <v>160.293015632576</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>0.138009949764872</v>
       </c>
-      <c r="E11" t="n">
-        <v>0.814305514065574</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="E12" t="n">
+        <v>0.404619300450722</v>
+      </c>
+      <c r="F12" t="n">
         <v>2495.43</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G12" t="n">
         <v>524364.15</v>
       </c>
+      <c r="H12" t="n">
+        <v>2.20491459947009</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>45331</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13" t="n">
+        <v>3919.605</v>
+      </c>
+      <c r="G13" t="n">
+        <v>539592.75</v>
+      </c>
+      <c r="H13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1032,143 +1180,238 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44452</v>
+        <v>44292</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>7.31312382905134</v>
+        <v>45.7971257985546</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0186472739593504</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1.09512941116791</v>
-      </c>
+        <v>0.0462709643091429</v>
+      </c>
+      <c r="E2"/>
       <c r="F2" t="n">
-        <v>13674.0471428571</v>
+        <v>5458.85785714287</v>
       </c>
       <c r="G2" t="n">
-        <v>7186340.60357143</v>
+        <v>3562871.65714287</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.6608382227856</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44517</v>
+        <v>44452</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>22.5234747698149</v>
+        <v>7.31312382905134</v>
       </c>
       <c r="D3" t="n">
-        <v>0.026820127000421</v>
+        <v>0.0186472739593504</v>
       </c>
       <c r="E3" t="n">
-        <v>1.15214486610791</v>
+        <v>0.479715570908414</v>
       </c>
       <c r="F3" t="n">
-        <v>11099.5307142857</v>
+        <v>13674.0471428571</v>
       </c>
       <c r="G3" t="n">
-        <v>11091201.1392857</v>
+        <v>7186340.60357143</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.864102927153004</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44589</v>
+        <v>44517</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>13.3793659977175</v>
+        <v>22.5234747698149</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0205672011357402</v>
+        <v>0.026820127000421</v>
       </c>
       <c r="E4" t="n">
-        <v>1.18605118392055</v>
+        <v>0.52563734835803</v>
       </c>
       <c r="F4" t="n">
-        <v>3737.09785714286</v>
+        <v>11099.5307142857</v>
       </c>
       <c r="G4" t="n">
-        <v>1835188.37142857</v>
+        <v>11091201.1392857</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.35263539137228</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44818</v>
+        <v>44589</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>80.2971338081475</v>
+        <v>13.3793659977175</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0756138674831853</v>
+        <v>0.0205672011357402</v>
       </c>
       <c r="E5" t="n">
-        <v>1.33613727954729</v>
+        <v>0.539502365829227</v>
       </c>
       <c r="F5" t="n">
-        <v>4981.49785714286</v>
+        <v>3737.09785714286</v>
       </c>
       <c r="G5" t="n">
-        <v>1686547.05</v>
+        <v>1835188.37142857</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.1264355341929</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44998</v>
+        <v>44666</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="n">
-        <v>73.3277604235412</v>
+        <v>8.55028667889765</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0601797177022106</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1.28317296907321</v>
-      </c>
+        <v>0.0127442482204935</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="n">
-        <v>6818.7</v>
+        <v>17543.2714285714</v>
       </c>
       <c r="G6" t="n">
-        <v>2266112.325</v>
+        <v>11838449.1321429</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.931980676245845</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
+        <v>44818</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>80.2971338081475</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0756138674831853</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.734125241659574</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4981.49785714286</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1686547.05</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.90470004349137</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>44998</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>73.3277604235412</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0601797177022106</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.604004404826991</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6818.7</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2266112.325</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.8652684209761</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>45140</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="n">
         <v>203.61423579318</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D9" t="n">
         <v>0.151213418262108</v>
       </c>
-      <c r="E7" t="n">
-        <v>1.47757506242285</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E9" t="n">
+        <v>0.861815715904159</v>
+      </c>
+      <c r="F9" t="n">
         <v>6875.74714285714</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G9" t="n">
         <v>682057.242857143</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2.30880813864651</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>45279</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>587.941323455919</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.116204075358259</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.08829296279805</v>
+      </c>
+      <c r="F10" t="n">
+        <v>2041.02</v>
+      </c>
+      <c r="G10" t="n">
+        <v>298589.7</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.7693339856495</v>
       </c>
     </row>
   </sheetData>
@@ -1207,13 +1450,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44285</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
         <v>218.653058116812</v>
@@ -1222,13 +1468,16 @@
         <v>0.0308372725815327</v>
       </c>
       <c r="E2" t="n">
-        <v>1.11553844289507</v>
+        <v>0.33357194499513</v>
       </c>
       <c r="F2" t="n">
         <v>5488.14642857143</v>
       </c>
       <c r="G2" t="n">
         <v>4876410.9</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.33975555583577</v>
       </c>
     </row>
     <row r="3">
@@ -1236,7 +1485,7 @@
         <v>44452</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
         <v>2.06639791095437</v>
@@ -1245,13 +1494,16 @@
         <v>0.028469917352607</v>
       </c>
       <c r="E3" t="n">
-        <v>0.813657725497269</v>
+        <v>0.103446523483956</v>
       </c>
       <c r="F3" t="n">
         <v>24196.695</v>
       </c>
       <c r="G3" t="n">
         <v>9603914.55</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.315213954111133</v>
       </c>
     </row>
     <row r="4">
@@ -1259,7 +1511,7 @@
         <v>44510</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="n">
         <v>56.4532973967771</v>
@@ -1268,13 +1520,16 @@
         <v>0.230530622192957</v>
       </c>
       <c r="E4" t="n">
-        <v>0.925645449472718</v>
+        <v>0.20838584321108</v>
       </c>
       <c r="F4" t="n">
         <v>7971.19071428572</v>
       </c>
       <c r="G4" t="n">
         <v>926679.107142858</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.75168931383232</v>
       </c>
     </row>
     <row r="5">
@@ -1282,7 +1537,7 @@
         <v>44589</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
         <v>4.20435343981279</v>
@@ -1291,7 +1546,7 @@
         <v>0.0173910258844274</v>
       </c>
       <c r="E5" t="n">
-        <v>0.857244517216307</v>
+        <v>0.114937829610508</v>
       </c>
       <c r="F5" t="n">
         <v>11892.435</v>
@@ -1299,97 +1554,136 @@
       <c r="G5" t="n">
         <v>9368415.675</v>
       </c>
+      <c r="H5" t="n">
+        <v>0.623699217943341</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44733</v>
+        <v>44659</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>5.84854833181856</v>
+        <v>45.7221685893927</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0217811972641943</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.838387320411005</v>
-      </c>
+        <v>0.0816494874119976</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="n">
-        <v>8549.13</v>
+        <v>6561.36857142857</v>
       </c>
       <c r="G6" t="n">
-        <v>3925004.625</v>
+        <v>1149150.76071429</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.66012682067494</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44806</v>
+        <v>44733</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>94.0961393698247</v>
+        <v>5.84854833181856</v>
       </c>
       <c r="D7" t="n">
-        <v>0.125964440018116</v>
+        <v>0.0217811972641943</v>
       </c>
       <c r="E7" t="n">
-        <v>1.03416328014474</v>
+        <v>0.118620701559585</v>
       </c>
       <c r="F7" t="n">
-        <v>6376.45714285715</v>
+        <v>8549.13</v>
       </c>
       <c r="G7" t="n">
-        <v>1543943.21785715</v>
+        <v>3925004.625</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.767048083224665</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44998</v>
+        <v>44806</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>4.110400422878</v>
+        <v>94.0961393698247</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0135347353218176</v>
+        <v>0.125964440018116</v>
       </c>
       <c r="E8" t="n">
-        <v>0.852390189325833</v>
+        <v>0.326952273525759</v>
       </c>
       <c r="F8" t="n">
-        <v>121642.65</v>
+        <v>6376.45714285715</v>
       </c>
       <c r="G8" t="n">
-        <v>139305352.5</v>
+        <v>1543943.21785715</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.97357180531061</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
+        <v>44998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.110400422878</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0135347353218176</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.14792716324069</v>
+      </c>
+      <c r="F9" t="n">
+        <v>121642.65</v>
+      </c>
+      <c r="G9" t="n">
+        <v>139305352.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.61388413160249</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>45279</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="n">
         <v>850.231688135016</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>-0.264707017120813</v>
       </c>
-      <c r="E9" t="n">
-        <v>1.23215856249894</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="E10" t="n">
+        <v>0.528260069853473</v>
+      </c>
+      <c r="F10" t="n">
         <v>1999.455</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>-105748.499999999</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.92953728708808</v>
       </c>
     </row>
   </sheetData>
@@ -1428,13 +1722,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44299</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="n">
         <v>201.556447682785</v>
@@ -1443,7 +1740,7 @@
         <v>0.0966260418499097</v>
       </c>
       <c r="E2" t="n">
-        <v>0.947540539626533</v>
+        <v>0.535718906702965</v>
       </c>
       <c r="F2" t="n">
         <v>1984.55571428571</v>
@@ -1451,97 +1748,162 @@
       <c r="G2" t="n">
         <v>626424.803571428</v>
       </c>
+      <c r="H2" t="n">
+        <v>2.30439669555911</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44452</v>
+        <v>44371</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>41.9734413050142</v>
+        <v>416.243786340365</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0482196240014123</v>
+        <v>0.214345900534267</v>
       </c>
       <c r="E3" t="n">
-        <v>0.954603621934516</v>
+        <v>0.89859430101436</v>
       </c>
       <c r="F3" t="n">
-        <v>14294.7535714286</v>
+        <v>3363.41357142857</v>
       </c>
       <c r="G3" t="n">
-        <v>4980376.03928571</v>
+        <v>643352.432142857</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.61934776344354</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44517</v>
+        <v>44452</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>61.6453450829362</v>
+        <v>41.9734413050142</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0396467471682954</v>
+        <v>0.0482196240014123</v>
       </c>
       <c r="E4" t="n">
-        <v>0.994357678715358</v>
+        <v>0.506400216436797</v>
       </c>
       <c r="F4" t="n">
-        <v>9733.09499999999</v>
+        <v>14294.7535714286</v>
       </c>
       <c r="G4" t="n">
-        <v>7413961.79999999</v>
+        <v>4980376.03928571</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.62297457746762</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44589</v>
+        <v>44517</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>18.3696008298861</v>
+        <v>61.6453450829362</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0240540549037401</v>
+        <v>0.0396467471682954</v>
       </c>
       <c r="E5" t="n">
-        <v>0.925241631392354</v>
+        <v>0.542257562907983</v>
       </c>
       <c r="F5" t="n">
-        <v>5443.77642857143</v>
+        <v>9733.09499999999</v>
       </c>
       <c r="G5" t="n">
-        <v>2896822.95</v>
+        <v>7413961.79999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.78990028805065</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
+        <v>44589</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="n">
+        <v>18.3696008298861</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0240540549037401</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.47259266099701</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5443.77642857143</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2896822.95</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.26409971922027</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>44666</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>43.1380098171326</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.026222037675287</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7" t="n">
+        <v>9272.565</v>
+      </c>
+      <c r="G7" t="n">
+        <v>14109328.5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.63486010494421</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>44818</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="n">
         <v>268.141444612033</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D8" t="n">
         <v>0.117343468865951</v>
       </c>
-      <c r="E6" t="n">
-        <v>1.29046111183131</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="E8" t="n">
+        <v>0.83771589530192</v>
+      </c>
+      <c r="F8" t="n">
         <v>2237.625</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G8" t="n">
         <v>444308.174999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.42836394481183</v>
       </c>
     </row>
   </sheetData>
@@ -1580,13 +1942,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44386</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
         <v>1661.73191635079</v>
@@ -1595,13 +1960,16 @@
         <v>0.387436294953374</v>
       </c>
       <c r="E2" t="n">
-        <v>1.72322186462555</v>
+        <v>0.843910837480766</v>
       </c>
       <c r="F2" t="n">
         <v>1203.56357142857</v>
       </c>
       <c r="G2" t="n">
         <v>178933.317857143</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.22056096130097</v>
       </c>
     </row>
     <row r="3">
@@ -1609,7 +1977,7 @@
         <v>44452</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" t="n">
         <v>25.6084522525835</v>
@@ -1618,13 +1986,16 @@
         <v>0.0748083206536477</v>
       </c>
       <c r="E3" t="n">
-        <v>0.929733787750404</v>
+        <v>0.0302828318577513</v>
       </c>
       <c r="F3" t="n">
         <v>11714.8821428571</v>
       </c>
       <c r="G3" t="n">
         <v>3774027.50357143</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.40838333096844</v>
       </c>
     </row>
     <row r="4">
@@ -1632,7 +2003,7 @@
         <v>44510</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
         <v>326.494767171751</v>
@@ -1641,13 +2012,16 @@
         <v>0.181034619271933</v>
       </c>
       <c r="E4" t="n">
-        <v>1.16430483770059</v>
+        <v>0.299044872433179</v>
       </c>
       <c r="F4" t="n">
         <v>4287.97071428572</v>
       </c>
       <c r="G4" t="n">
         <v>959279.58214286</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2.51387622510069</v>
       </c>
     </row>
     <row r="5">
@@ -1655,7 +2029,7 @@
         <v>44589</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="n">
         <v>55.2594896825599</v>
@@ -1664,7 +2038,7 @@
         <v>0.0466003004043193</v>
       </c>
       <c r="E5" t="n">
-        <v>0.95598794379407</v>
+        <v>0.0701437122950006</v>
       </c>
       <c r="F5" t="n">
         <v>3619.28785714286</v>
@@ -1672,97 +2046,212 @@
       <c r="G5" t="n">
         <v>1654299.02142857</v>
       </c>
+      <c r="H5" t="n">
+        <v>1.74240686992049</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44733</v>
+        <v>44659</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>19.3061500671871</v>
+        <v>-59.2075325514556</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0247248402753767</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.878364493092622</v>
-      </c>
+        <v>0.00694043951640586</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="n">
-        <v>20718.7864285714</v>
+        <v>-20267.6914285714</v>
       </c>
       <c r="G6" t="n">
-        <v>24301261.3928571</v>
+        <v>-90527182.4357143</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44806</v>
+        <v>44733</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>83.4160791046595</v>
+        <v>19.3061500671871</v>
       </c>
       <c r="D7" t="n">
-        <v>0.104270024651914</v>
+        <v>0.0247248402753767</v>
       </c>
       <c r="E7" t="n">
-        <v>1.12718696043453</v>
+        <v>0.00399777034402538</v>
       </c>
       <c r="F7" t="n">
-        <v>11988.0964285714</v>
+        <v>20718.7864285714</v>
       </c>
       <c r="G7" t="n">
-        <v>4242453.76071428</v>
+        <v>24301261.3928571</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.28569567764907</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44959</v>
+        <v>44806</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>30.1205661719794</v>
+        <v>83.4160791046595</v>
       </c>
       <c r="D8" t="n">
-        <v>0.017179789481342</v>
+        <v>0.104270024651914</v>
       </c>
       <c r="E8" t="n">
-        <v>0.994350520519222</v>
+        <v>0.290215285645218</v>
       </c>
       <c r="F8" t="n">
-        <v>6639.98142857143</v>
+        <v>11988.0964285714</v>
       </c>
       <c r="G8" t="n">
-        <v>10435488.675</v>
+        <v>4242453.76071428</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.92124977238071</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
+        <v>44879</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="n">
+        <v>62.1041048151678</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0624314324451668</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9" t="n">
+        <v>7245.89785714286</v>
+      </c>
+      <c r="G9" t="n">
+        <v>3017604.06428571</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.79312030612925</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>44959</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="n">
+        <v>30.1205661719794</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.017179789481342</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.101064998910301</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6639.98142857143</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10435488.675</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.47886313097672</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
         <v>44999</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="n">
         <v>203.383280877396</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D11" t="n">
         <v>0.223866557705922</v>
       </c>
-      <c r="E9" t="n">
-        <v>1.16293097131649</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="E11" t="n">
+        <v>0.292879350342034</v>
+      </c>
+      <c r="F11" t="n">
         <v>2950.095</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G11" t="n">
         <v>466498.274999997</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2.30831524887617</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7.12054440834328</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0106085660132641</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0222071233915194</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7021.935</v>
+      </c>
+      <c r="G12" t="n">
+        <v>16680177.3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.852513199325168</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>45279</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1159.08432338453</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.192383869915185</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.69658739105357</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3105.9</v>
+      </c>
+      <c r="G13" t="n">
+        <v>613482.825</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3.06411503203648</v>
       </c>
     </row>
   </sheetData>
@@ -1801,13 +2290,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44299</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
         <v>23.3064027849153</v>
@@ -1816,13 +2308,16 @@
         <v>0.0288993102026876</v>
       </c>
       <c r="E2" t="n">
-        <v>0.235947559167846</v>
+        <v>0.346751698763138</v>
       </c>
       <c r="F2" t="n">
         <v>4290.66642857143</v>
       </c>
       <c r="G2" t="n">
         <v>2672451.18214286</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1.36747524772831</v>
       </c>
     </row>
     <row r="3">
@@ -1830,7 +2325,7 @@
         <v>44386</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="n">
         <v>270.901397309407</v>
@@ -1839,13 +2334,16 @@
         <v>0.233297132170326</v>
       </c>
       <c r="E3" t="n">
-        <v>3.00425309577892</v>
+        <v>2.32073631840445</v>
       </c>
       <c r="F3" t="n">
         <v>3691.38</v>
       </c>
       <c r="G3" t="n">
         <v>424047.15</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.43281124512988</v>
       </c>
     </row>
     <row r="4">
@@ -1853,7 +2351,7 @@
         <v>44452</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="n">
         <v>2.04807802379181</v>
@@ -1862,7 +2360,7 @@
         <v>0.0334046106509795</v>
       </c>
       <c r="E4" t="n">
-        <v>1.11679553298501</v>
+        <v>0.478400138466944</v>
       </c>
       <c r="F4" t="n">
         <v>24413.1324193548</v>
@@ -1870,74 +2368,162 @@
       <c r="G4" t="n">
         <v>4019571.72048387</v>
       </c>
+      <c r="H4" t="n">
+        <v>0.311346497546363</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44659</v>
+        <v>44510</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>10.1562152863735</v>
+        <v>21.1919407049499</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0160991553702436</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1.20205744593307</v>
-      </c>
+        <v>0.0277510769684758</v>
+      </c>
+      <c r="E5"/>
       <c r="F5" t="n">
-        <v>19692.375</v>
+        <v>9437.55</v>
       </c>
       <c r="G5" t="n">
-        <v>12231930.525</v>
+        <v>5271219.75</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.32617073013491</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44806</v>
+        <v>44589</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>35.2877784497159</v>
+        <v>138.347849975591</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0598939505762173</v>
+        <v>0.00958213989251452</v>
       </c>
       <c r="E6" t="n">
-        <v>1.21757509060473</v>
+        <v>0.455538766986625</v>
       </c>
       <c r="F6" t="n">
-        <v>22670.7385714286</v>
+        <v>722.815714285718</v>
       </c>
       <c r="G6" t="n">
-        <v>9576420.99642858</v>
+        <v>618555.867857144</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.14097241428295</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
+        <v>44659</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="n">
+        <v>10.1562152863735</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0160991553702436</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.554925263836542</v>
+      </c>
+      <c r="F7" t="n">
+        <v>19692.375</v>
+      </c>
+      <c r="G7" t="n">
+        <v>12231930.525</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.00673189825654</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>44806</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="n">
+        <v>35.2877784497159</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0598939505762173</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.578650992377742</v>
+      </c>
+      <c r="F8" t="n">
+        <v>22670.7385714286</v>
+      </c>
+      <c r="G8" t="n">
+        <v>9576420.99642858</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.54762431811064</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>45140</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="n">
+        <v>139.040343548826</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.114325713526605</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.603687349344395</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6113.33357142857</v>
+      </c>
+      <c r="G9" t="n">
+        <v>962513.164285714</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2.14314083218554</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>45197</v>
       </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="n">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="n">
         <v>18.5478970626159</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D10" t="n">
         <v>0.0380123901994629</v>
       </c>
-      <c r="E7" t="n">
-        <v>1.19617447962169</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E10" t="n">
+        <v>0.46420761962736</v>
+      </c>
+      <c r="F10" t="n">
         <v>10782.8935714286</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G10" t="n">
         <v>5673357.30000001</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.26829467697673</v>
       </c>
     </row>
   </sheetData>
@@ -1976,13 +2562,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44292</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
         <v>1474.27392009435</v>
@@ -1991,13 +2580,16 @@
         <v>0.609595398242257</v>
       </c>
       <c r="E2" t="n">
-        <v>0.588459099645472</v>
+        <v>0.642692214475338</v>
       </c>
       <c r="F2" t="n">
         <v>1356.6</v>
       </c>
       <c r="G2" t="n">
         <v>111270.525</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.16857818293498</v>
       </c>
     </row>
     <row r="3">
@@ -2005,7 +2597,7 @@
         <v>44452</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
         <v>163.514515592335</v>
@@ -2014,13 +2606,16 @@
         <v>0.19909322659857</v>
       </c>
       <c r="E3" t="n">
-        <v>1.05548560188029</v>
+        <v>0.456852129234562</v>
       </c>
       <c r="F3" t="n">
         <v>6115.665</v>
       </c>
       <c r="G3" t="n">
         <v>1170340.35</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.21355631211454</v>
       </c>
     </row>
     <row r="4">
@@ -2028,7 +2623,7 @@
         <v>44589</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="n">
         <v>65.6511558308027</v>
@@ -2037,13 +2632,16 @@
         <v>0.09276270132275</v>
       </c>
       <c r="E4" t="n">
-        <v>1.01102869478466</v>
+        <v>0.387986636389939</v>
       </c>
       <c r="F4" t="n">
         <v>7616.01214285714</v>
       </c>
       <c r="G4" t="n">
         <v>2101813.63928571</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.81724237652635</v>
       </c>
     </row>
     <row r="5">
@@ -2051,7 +2649,7 @@
         <v>44665</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="n">
         <v>33.6536236839781</v>
@@ -2060,13 +2658,16 @@
         <v>0.132219643097552</v>
       </c>
       <c r="E5" t="n">
-        <v>0.907178487084247</v>
+        <v>0.317426441464453</v>
       </c>
       <c r="F5" t="n">
         <v>17828.6892857143</v>
       </c>
       <c r="G5" t="n">
         <v>3640719.33214286</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.5270318341239</v>
       </c>
     </row>
     <row r="6">
@@ -2074,7 +2675,7 @@
         <v>44817</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="n">
         <v>1147.67621184873</v>
@@ -2083,13 +2684,16 @@
         <v>0.370207050897618</v>
       </c>
       <c r="E6" t="n">
-        <v>1.43410908639999</v>
+        <v>0.810269715804584</v>
       </c>
       <c r="F6" t="n">
         <v>1394.12142857143</v>
       </c>
       <c r="G6" t="n">
         <v>158539.692857143</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3.05981938001173</v>
       </c>
     </row>
     <row r="7">
@@ -2097,7 +2701,7 @@
         <v>44880</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="n">
         <v>20.7914719322554</v>
@@ -2106,13 +2710,16 @@
         <v>0.108285591446864</v>
       </c>
       <c r="E7" t="n">
-        <v>0.684173748145478</v>
+        <v>0.252628149252128</v>
       </c>
       <c r="F7" t="n">
         <v>9619.32857142857</v>
       </c>
       <c r="G7" t="n">
         <v>1687826.05714286</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1.31788523629769</v>
       </c>
     </row>
     <row r="8">
@@ -2120,7 +2727,7 @@
         <v>44953</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="n">
         <v>5.13894891976541</v>
@@ -2129,13 +2736,16 @@
         <v>0.0176083819768147</v>
       </c>
       <c r="E8" t="n">
-        <v>1.13760053883744</v>
+        <v>0.371862313459475</v>
       </c>
       <c r="F8" t="n">
         <v>19459.2321428571</v>
       </c>
       <c r="G8" t="n">
         <v>27627797.0464286</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.710874300897029</v>
       </c>
     </row>
     <row r="9">
@@ -2143,7 +2753,7 @@
         <v>44998</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="n">
         <v>33.1790704053949</v>
@@ -2152,13 +2762,16 @@
         <v>0.0942639400766061</v>
       </c>
       <c r="E9" t="n">
-        <v>1.2351274384367</v>
+        <v>0.463727151545212</v>
       </c>
       <c r="F9" t="n">
         <v>18083.6892857143</v>
       </c>
       <c r="G9" t="n">
         <v>4604184.19285714</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.52086421401315</v>
       </c>
     </row>
     <row r="10">
@@ -2166,7 +2779,7 @@
         <v>45140</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
         <v>657.928746316773</v>
@@ -2175,13 +2788,16 @@
         <v>-0.624858780565361</v>
       </c>
       <c r="E10" t="n">
-        <v>1.70007552742378</v>
+        <v>0.912353238191325</v>
       </c>
       <c r="F10" t="n">
         <v>1823.90571428572</v>
       </c>
       <c r="G10" t="n">
         <v>-61297.0821428564</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.81817886206828</v>
       </c>
     </row>
     <row r="11">
@@ -2189,7 +2805,7 @@
         <v>45197</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="n">
         <v>133.328381136318</v>
@@ -2198,13 +2814,16 @@
         <v>0.0966021881464723</v>
       </c>
       <c r="E11" t="n">
-        <v>1.38542489812252</v>
+        <v>0.613572526993539</v>
       </c>
       <c r="F11" t="n">
         <v>750.027857142865</v>
       </c>
       <c r="G11" t="n">
         <v>273295.885714292</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2.12492260596996</v>
       </c>
     </row>
     <row r="12">
@@ -2212,7 +2831,7 @@
         <v>45231</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="n">
         <v>17.3551452799212</v>
@@ -2221,13 +2840,16 @@
         <v>0.0456410932698102</v>
       </c>
       <c r="E12" t="n">
-        <v>1.2714292155857</v>
+        <v>0.465127438436695</v>
       </c>
       <c r="F12" t="n">
         <v>2880.99</v>
       </c>
       <c r="G12" t="n">
         <v>1527569.85</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.23942825350176</v>
       </c>
     </row>
     <row r="13">
@@ -2235,7 +2857,7 @@
         <v>45296</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="n">
         <v>236.595392304735</v>
@@ -2244,7 +2866,7 @@
         <v>0.229962718506469</v>
       </c>
       <c r="E13" t="n">
-        <v>1.46778642648194</v>
+        <v>0.550454897727977</v>
       </c>
       <c r="F13" t="n">
         <v>2535.975</v>
@@ -2252,6 +2874,27 @@
       <c r="G13" t="n">
         <v>628582.649999999</v>
       </c>
+      <c r="H13" t="n">
+        <v>2.37400628248923</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>45331</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14" t="n">
+        <v>47179.08</v>
+      </c>
+      <c r="G14" t="n">
+        <v>17329386.9</v>
+      </c>
+      <c r="H14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2289,13 +2932,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44292</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="n">
         <v>79.9725579879591</v>
@@ -2304,7 +2950,7 @@
         <v>0.0836415522456026</v>
       </c>
       <c r="E2" t="n">
-        <v>0.391831821845463</v>
+        <v>0.175235931608227</v>
       </c>
       <c r="F2" t="n">
         <v>2500.85785714285</v>
@@ -2312,97 +2958,188 @@
       <c r="G2" t="n">
         <v>774402.396428567</v>
       </c>
+      <c r="H2" t="n">
+        <v>1.90294098750518</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44452</v>
+        <v>44371</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>14.3008118570891</v>
+        <v>97.517092917943</v>
       </c>
       <c r="D3" t="n">
-        <v>0.10472695502504</v>
+        <v>0.0844166976160872</v>
       </c>
       <c r="E3" t="n">
-        <v>0.999480006838803</v>
+        <v>0.428172659072591</v>
       </c>
       <c r="F3" t="n">
-        <v>13985.22</v>
+        <v>12305.535</v>
       </c>
       <c r="G3" t="n">
-        <v>1949681.55</v>
+        <v>5685082.2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.9890807460505</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44589</v>
+        <v>44452</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>6.79493167987407</v>
+        <v>14.3008118570891</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0279077813421051</v>
+        <v>0.10472695502504</v>
       </c>
       <c r="E4" t="n">
-        <v>1.01485820994369</v>
+        <v>0.227107949809334</v>
       </c>
       <c r="F4" t="n">
-        <v>14716.8514285714</v>
+        <v>13985.22</v>
       </c>
       <c r="G4" t="n">
-        <v>4798781.61428571</v>
+        <v>1949681.55</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.15536069306266</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44818</v>
+        <v>44517</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="n">
-        <v>52.7801968701343</v>
+        <v>19.273719443755</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0490018181170012</v>
+        <v>0.0768117708525735</v>
       </c>
       <c r="E5" t="n">
-        <v>1.15128049983373</v>
+        <v>0.258943438038391</v>
       </c>
       <c r="F5" t="n">
-        <v>7578.6</v>
+        <v>10376.8242857143</v>
       </c>
       <c r="G5" t="n">
-        <v>3433442.4</v>
+        <v>2877506.33571429</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.28496553292348</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
+        <v>44589</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6.79493167987407</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0279077813421051</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.21984313155044</v>
+      </c>
+      <c r="F6" t="n">
+        <v>14716.8514285714</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4798781.61428571</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.832185094445576</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>44665</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="n">
+        <v>5.52548180523963</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0835954778785003</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7" t="n">
+        <v>18097.9692857143</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2641234.08214286</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.74237015316871</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>44818</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>52.7801968701343</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0490018181170012</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.346273489592434</v>
+      </c>
+      <c r="F8" t="n">
+        <v>7578.6</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3433442.4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.72247100580547</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
         <v>45279</v>
       </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="n">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="n">
         <v>409.296138546743</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D9" t="n">
         <v>0.0895346799829791</v>
       </c>
-      <c r="E6" t="n">
-        <v>1.36819286547664</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="E9" t="n">
+        <v>0.686132065900496</v>
+      </c>
+      <c r="F9" t="n">
         <v>1954.575</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G9" t="n">
         <v>458437.725</v>
+      </c>
+      <c r="H9" t="n">
+        <v>2.61203764736759</v>
       </c>
     </row>
   </sheetData>
@@ -2441,13 +3178,16 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>44292</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
         <v>110.528991754537</v>
@@ -2456,7 +3196,7 @@
         <v>0.0578152666505854</v>
       </c>
       <c r="E2" t="n">
-        <v>0.871378375484023</v>
+        <v>0.334368448888413</v>
       </c>
       <c r="F2" t="n">
         <v>2261.85</v>
@@ -2464,166 +3204,216 @@
       <c r="G2" t="n">
         <v>1490548.95</v>
       </c>
+      <c r="H2" t="n">
+        <v>2.04347620840636</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44452</v>
+        <v>44371</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" t="n">
-        <v>19.0713037906123</v>
+        <v>145.543610583516</v>
       </c>
       <c r="D3" t="n">
-        <v>0.111120888231963</v>
+        <v>0.0876716470388422</v>
       </c>
       <c r="E3" t="n">
-        <v>0.875693725023813</v>
+        <v>0.432978589290512</v>
       </c>
       <c r="F3" t="n">
-        <v>7865.22</v>
+        <v>4122.47571428571</v>
       </c>
       <c r="G3" t="n">
-        <v>1033398.975</v>
+        <v>1650464.00357143</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2.16299314451045</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44517</v>
+        <v>44452</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>16.9350140609002</v>
+        <v>19.0713037906123</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0463166323010258</v>
+        <v>0.111120888231963</v>
       </c>
       <c r="E4" t="n">
-        <v>0.861109604946484</v>
+        <v>0.237758928017856</v>
       </c>
       <c r="F4" t="n">
-        <v>11809.8514285714</v>
+        <v>7865.22</v>
       </c>
       <c r="G4" t="n">
-        <v>10479710.4107143</v>
+        <v>1033398.975</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.28038038416888</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44589</v>
+        <v>44517</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>4.49444319884161</v>
+        <v>16.9350140609002</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0437964783271548</v>
+        <v>0.0463166323010258</v>
       </c>
       <c r="E5" t="n">
-        <v>0.829087949994082</v>
+        <v>0.218569566722467</v>
       </c>
       <c r="F5" t="n">
-        <v>11124.8485714286</v>
+        <v>11809.8514285714</v>
       </c>
       <c r="G5" t="n">
-        <v>2159105.4</v>
+        <v>10479710.4107143</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1.2287855615693</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44666</v>
+        <v>44589</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>2.89214023293876</v>
+        <v>4.49444319884161</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0252018268584692</v>
+        <v>0.0437964783271548</v>
       </c>
       <c r="E6" t="n">
-        <v>0.631433198623971</v>
+        <v>0.184070989202584</v>
       </c>
       <c r="F6" t="n">
-        <v>17288.235</v>
+        <v>11124.8485714286</v>
       </c>
       <c r="G6" t="n">
-        <v>11318857.125</v>
+        <v>2159105.4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.652675896147369</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44818</v>
+        <v>44666</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>105.628429740967</v>
+        <v>2.89214023293876</v>
       </c>
       <c r="D7" t="n">
-        <v>0.142353917790553</v>
+        <v>0.0252018268584692</v>
       </c>
       <c r="E7" t="n">
-        <v>1.04927645855292</v>
+        <v>0.14985963462285</v>
       </c>
       <c r="F7" t="n">
-        <v>7573.71857142857</v>
+        <v>17288.235</v>
       </c>
       <c r="G7" t="n">
-        <v>2255825.98928571</v>
+        <v>11318857.125</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.461219347030154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44966</v>
+        <v>44818</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>8.00184819830957</v>
+        <v>105.628429740967</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0131382698505472</v>
+        <v>0.142353917790553</v>
       </c>
       <c r="E8" t="n">
-        <v>0.778096370738196</v>
+        <v>0.398722933657988</v>
       </c>
       <c r="F8" t="n">
-        <v>6248.55642857143</v>
+        <v>7573.71857142857</v>
       </c>
       <c r="G8" t="n">
-        <v>6658394.97857143</v>
+        <v>2255825.98928571</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2.02378082367035</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
+        <v>44966</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8.00184819830957</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0131382698505472</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.110956390662781</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6248.55642857143</v>
+      </c>
+      <c r="G9" t="n">
+        <v>6658394.97857143</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.903190308194961</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>44998</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="n">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="n">
         <v>126.543034122329</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>0.154867311917387</v>
       </c>
-      <c r="E9" t="n">
-        <v>1.09144358834172</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="E10" t="n">
+        <v>0.327003484688787</v>
+      </c>
+      <c r="F10" t="n">
         <v>3951.225</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>714381.225</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.10223824332676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rolling down the river
</commit_message>
<xml_diff>
--- a/04_Output/rC_DG.xlsx
+++ b/04_Output/rC_DG.xlsx
@@ -510,7 +510,7 @@
         <v>0.292536199651649</v>
       </c>
       <c r="E4" t="n">
-        <v>0.491693805811854</v>
+        <v>0.556155956335123</v>
       </c>
       <c r="F4" t="n">
         <v>3847.36714285714</v>
@@ -522,7 +522,7 @@
         <v>2.71586636394285</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.308305262766735</v>
+        <v>-0.254803407197853</v>
       </c>
     </row>
     <row r="5">
@@ -589,7 +589,7 @@
         <v>0.0406457351860475</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0569027203963497</v>
+        <v>0.0569053265008198</v>
       </c>
       <c r="F7" t="n">
         <v>34805.3871428571</v>
@@ -601,7 +601,7 @@
         <v>0.458353531187161</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.24486697042599</v>
+        <v>-1.24484708050043</v>
       </c>
     </row>
     <row r="8">
@@ -618,7 +618,7 @@
         <v>0.194918677610752</v>
       </c>
       <c r="E8" t="n">
-        <v>0.326424187469587</v>
+        <v>0.326470276576917</v>
       </c>
       <c r="F8" t="n">
         <v>2774.655</v>
@@ -630,7 +630,7 @@
         <v>2.45988099625789</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.486217668253406</v>
+        <v>-0.486156352846017</v>
       </c>
     </row>
     <row r="9">
@@ -647,7 +647,7 @@
         <v>0.0351128684887311</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0913046673568094</v>
+        <v>0.0868903014673715</v>
       </c>
       <c r="F9" t="n">
         <v>22291.3714285714</v>
@@ -659,7 +659,7 @@
         <v>1.0498032203381</v>
       </c>
       <c r="I9" t="n">
-        <v>-1.03950702141972</v>
+        <v>-1.06102869598244</v>
       </c>
     </row>
     <row r="10">
@@ -676,7 +676,7 @@
         <v>0.0129171130222743</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0686781937579025</v>
+        <v>0.0689949376511942</v>
       </c>
       <c r="F10" t="n">
         <v>16770.8035714286</v>
@@ -688,7 +688,7 @@
         <v>0.474416132053351</v>
       </c>
       <c r="I10" t="n">
-        <v>-1.16318113534122</v>
+        <v>-1.16118277347733</v>
       </c>
     </row>
     <row r="11">
@@ -705,7 +705,7 @@
         <v>0.115971738074685</v>
       </c>
       <c r="E11" t="n">
-        <v>0.143757202817436</v>
+        <v>0.141394155033208</v>
       </c>
       <c r="F11" t="n">
         <v>4863.83357142857</v>
@@ -717,7 +717,7 @@
         <v>1.48911255303911</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.842370386182687</v>
+        <v>-0.849568543080074</v>
       </c>
     </row>
     <row r="12">
@@ -734,7 +734,7 @@
         <v>0.0391666376832519</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0770005487413572</v>
+        <v>0.0770541272743987</v>
       </c>
       <c r="F12" t="n">
         <v>9153.26142857143</v>
@@ -746,7 +746,7 @@
         <v>0.737394137804323</v>
       </c>
       <c r="I12" t="n">
-        <v>-1.11350617983409</v>
+        <v>-1.11320409407092</v>
       </c>
     </row>
     <row r="13">
@@ -763,7 +763,7 @@
         <v>0.145089110762292</v>
       </c>
       <c r="E13" t="n">
-        <v>0.19325455560002</v>
+        <v>0.188932431571157</v>
       </c>
       <c r="F13" t="n">
         <v>11023.5042857143</v>
@@ -775,7 +775,7 @@
         <v>1.73583157510342</v>
       </c>
       <c r="I13" t="n">
-        <v>-0.713870259641819</v>
+        <v>-0.723693485998537</v>
       </c>
     </row>
     <row r="14">
@@ -792,7 +792,7 @@
         <v>0.0366654380801947</v>
       </c>
       <c r="E14" t="n">
-        <v>0.038709265448834</v>
+        <v>0.0388449810466055</v>
       </c>
       <c r="F14" t="n">
         <v>24529.9435714286</v>
@@ -804,7 +804,7 @@
         <v>0.309273455177549</v>
       </c>
       <c r="I14" t="n">
-        <v>-1.41218506982144</v>
+        <v>-1.41066508611846</v>
       </c>
     </row>
     <row r="15">
@@ -893,7 +893,7 @@
         <v>0.0308372725815327</v>
       </c>
       <c r="E2" t="n">
-        <v>0.344292899072056</v>
+        <v>0.33357194499513</v>
       </c>
       <c r="F2" t="n">
         <v>5488.14642857143</v>
@@ -905,7 +905,7 @@
         <v>2.33975555583577</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.463071934383983</v>
+        <v>-0.476810482753012</v>
       </c>
     </row>
     <row r="3">
@@ -922,7 +922,7 @@
         <v>0.028469917352607</v>
       </c>
       <c r="E3" t="n">
-        <v>0.103446523483956</v>
+        <v>0.103246752096473</v>
       </c>
       <c r="F3" t="n">
         <v>24196.695</v>
@@ -934,7 +934,7 @@
         <v>0.315213954111133</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.985284100040337</v>
+        <v>-0.986123601354522</v>
       </c>
     </row>
     <row r="4">
@@ -951,7 +951,7 @@
         <v>0.230530622192957</v>
       </c>
       <c r="E4" t="n">
-        <v>0.20838584321108</v>
+        <v>0.208368019852923</v>
       </c>
       <c r="F4" t="n">
         <v>7971.19071428572</v>
@@ -963,7 +963,7 @@
         <v>1.75168931383232</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.681131788367453</v>
+        <v>-0.681168935406929</v>
       </c>
     </row>
     <row r="5">
@@ -980,7 +980,7 @@
         <v>0.0173910258844274</v>
       </c>
       <c r="E5" t="n">
-        <v>0.114937829610508</v>
+        <v>0.115660292693498</v>
       </c>
       <c r="F5" t="n">
         <v>11892.435</v>
@@ -992,7 +992,7 @@
         <v>0.623699217943341</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.93953700797733</v>
+        <v>-0.936815712992044</v>
       </c>
     </row>
     <row r="6">
@@ -1034,7 +1034,7 @@
         <v>0.0217811972641943</v>
       </c>
       <c r="E7" t="n">
-        <v>0.118623158203254</v>
+        <v>0.118618295568362</v>
       </c>
       <c r="F7" t="n">
         <v>8549.13</v>
@@ -1046,7 +1046,7 @@
         <v>0.767048083224665</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.925830517564636</v>
+        <v>-0.925848320654844</v>
       </c>
     </row>
     <row r="8">
@@ -1063,7 +1063,7 @@
         <v>0.125964440018116</v>
       </c>
       <c r="E8" t="n">
-        <v>0.326952273525759</v>
+        <v>0.32669127366084</v>
       </c>
       <c r="F8" t="n">
         <v>6376.45714285715</v>
@@ -1075,7 +1075,7 @@
         <v>1.97357180531061</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.485515638340187</v>
+        <v>-0.485862465927253</v>
       </c>
     </row>
     <row r="9">
@@ -1092,7 +1092,7 @@
         <v>0.0135347353218176</v>
       </c>
       <c r="E9" t="n">
-        <v>0.14792716324069</v>
+        <v>0.148399542142312</v>
       </c>
       <c r="F9" t="n">
         <v>121642.65</v>
@@ -1104,7 +1104,7 @@
         <v>0.61388413160249</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.829952071017485</v>
+        <v>-0.828567438985388</v>
       </c>
     </row>
     <row r="10">
@@ -1464,7 +1464,7 @@
         <v>0.0748083206536477</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0302828318577513</v>
+        <v>0.0314608700934574</v>
       </c>
       <c r="F3" t="n">
         <v>11714.8821428571</v>
@@ -1476,7 +1476,7 @@
         <v>1.40838333096844</v>
       </c>
       <c r="I3" t="n">
-        <v>-1.51880351481632</v>
+        <v>-1.50222927053785</v>
       </c>
     </row>
     <row r="4">
@@ -1493,7 +1493,7 @@
         <v>0.181034619271933</v>
       </c>
       <c r="E4" t="n">
-        <v>0.29923926144503</v>
+        <v>0.298854491442191</v>
       </c>
       <c r="F4" t="n">
         <v>4287.97071428572</v>
@@ -1505,7 +1505,7 @@
         <v>2.51387622510069</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.523981425813272</v>
+        <v>-0.524540212830461</v>
       </c>
     </row>
     <row r="5">
@@ -1522,7 +1522,7 @@
         <v>0.0466003004043193</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0701437122950006</v>
+        <v>0.071022433807391</v>
       </c>
       <c r="F5" t="n">
         <v>3619.28785714286</v>
@@ -1534,7 +1534,7 @@
         <v>1.74240686992049</v>
       </c>
       <c r="I5" t="n">
-        <v>-1.15401125318833</v>
+        <v>-1.1486044493111</v>
       </c>
     </row>
     <row r="6">
@@ -1576,7 +1576,7 @@
         <v>0.0247248402753767</v>
       </c>
       <c r="E7" t="n">
-        <v>0.00399777034402538</v>
+        <v>0.00408688713481306</v>
       </c>
       <c r="F7" t="n">
         <v>20718.7864285714</v>
@@ -1588,7 +1588,7 @@
         <v>1.28569567764907</v>
       </c>
       <c r="I7" t="n">
-        <v>-2.3981821579886</v>
+        <v>-2.38860735578112</v>
       </c>
     </row>
     <row r="8">
@@ -1605,7 +1605,7 @@
         <v>0.104270024651914</v>
       </c>
       <c r="E8" t="n">
-        <v>0.290562952226383</v>
+        <v>0.292886326762752</v>
       </c>
       <c r="F8" t="n">
         <v>11988.0964285714</v>
@@ -1617,7 +1617,7 @@
         <v>1.92124977238071</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.536759760545043</v>
+        <v>-0.533300902644435</v>
       </c>
     </row>
     <row r="9">
@@ -1663,7 +1663,7 @@
         <v>0.017179789481342</v>
       </c>
       <c r="E10" t="n">
-        <v>0.101064998910301</v>
+        <v>0.100905322589866</v>
       </c>
       <c r="F10" t="n">
         <v>6639.98142857143</v>
@@ -1675,7 +1675,7 @@
         <v>1.47886313097672</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.995399224349649</v>
+        <v>-0.996085924838993</v>
       </c>
     </row>
     <row r="11">
@@ -1692,7 +1692,7 @@
         <v>0.223866557705922</v>
       </c>
       <c r="E11" t="n">
-        <v>0.292879350342034</v>
+        <v>0.292268158933349</v>
       </c>
       <c r="F11" t="n">
         <v>2950.095</v>
@@ -1704,7 +1704,7 @@
         <v>2.30831524887617</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.533311247467084</v>
+        <v>-0.534218496147122</v>
       </c>
     </row>
     <row r="12">
@@ -1721,7 +1721,7 @@
         <v>0.0106085660132641</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0435957774013449</v>
+        <v>0.0398067631956158</v>
       </c>
       <c r="F12" t="n">
         <v>7021.935</v>
@@ -1733,7 +1733,7 @@
         <v>0.852513199325168</v>
       </c>
       <c r="I12" t="n">
-        <v>-1.36055557357783</v>
+        <v>-1.40004313473525</v>
       </c>
     </row>
     <row r="13">
@@ -1984,7 +1984,7 @@
         <v>0.0598939505762173</v>
       </c>
       <c r="E8" t="n">
-        <v>0.578650992377742</v>
+        <v>0.578629035198701</v>
       </c>
       <c r="F8" t="n">
         <v>22670.7385714286</v>
@@ -1996,7 +1996,7 @@
         <v>1.54762431811064</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.23758329773181</v>
+        <v>-0.237599777549088</v>
       </c>
     </row>
     <row r="9">
@@ -2143,7 +2143,7 @@
         <v>0.19909322659857</v>
       </c>
       <c r="E3" t="n">
-        <v>0.456852129234562</v>
+        <v>0.456824240921209</v>
       </c>
       <c r="F3" t="n">
         <v>6115.665</v>
@@ -2155,7 +2155,7 @@
         <v>2.21355631211454</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.340224346646562</v>
+        <v>-0.340250858748654</v>
       </c>
     </row>
     <row r="4">
@@ -2172,7 +2172,7 @@
         <v>0.09276270132275</v>
       </c>
       <c r="E4" t="n">
-        <v>0.387986636389939</v>
+        <v>0.38887615975603</v>
       </c>
       <c r="F4" t="n">
         <v>7616.01214285714</v>
@@ -2184,7 +2184,7 @@
         <v>1.81724237652635</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.41118323276161</v>
+        <v>-0.410188680672972</v>
       </c>
     </row>
     <row r="5">
@@ -2230,7 +2230,7 @@
         <v>0.370207050897618</v>
       </c>
       <c r="E6" t="n">
-        <v>0.810018775061474</v>
+        <v>0.810515482511753</v>
       </c>
       <c r="F6" t="n">
         <v>1394.12142857143</v>
@@ -2242,7 +2242,7 @@
         <v>3.05981938001173</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0915049146878972</v>
+        <v>-0.0912386848189221</v>
       </c>
     </row>
     <row r="7">
@@ -2284,7 +2284,7 @@
         <v>0.0176083819768147</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0508658047240336</v>
+        <v>-0.0509851313580177</v>
       </c>
       <c r="F8" t="n">
         <v>19459.2321428571</v>
@@ -2313,7 +2313,7 @@
         <v>0.0942639400766061</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0409990333617032</v>
+        <v>0.0410550448373626</v>
       </c>
       <c r="F9" t="n">
         <v>18083.6892857143</v>
@@ -2325,7 +2325,7 @@
         <v>1.52086421401315</v>
       </c>
       <c r="I9" t="n">
-        <v>-1.38722638256385</v>
+        <v>-1.38663346922879</v>
       </c>
     </row>
     <row r="10">
@@ -2371,7 +2371,7 @@
         <v>0.0966021881464723</v>
       </c>
       <c r="E11" t="n">
-        <v>0.19084440881003</v>
+        <v>0.190986898896875</v>
       </c>
       <c r="F11" t="n">
         <v>750.027857142865</v>
@@ -2383,7 +2383,7 @@
         <v>2.12492260596996</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.719320559102468</v>
+        <v>-0.718996422971846</v>
       </c>
     </row>
     <row r="12">
@@ -2400,7 +2400,7 @@
         <v>0.0456410932698102</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0833480434549802</v>
+        <v>0.0829762877707573</v>
       </c>
       <c r="F12" t="n">
         <v>2880.99</v>
@@ -2412,7 +2412,7 @@
         <v>1.23942825350176</v>
       </c>
       <c r="I12" t="n">
-        <v>-1.07910459051719</v>
+        <v>-1.08104599872781</v>
       </c>
     </row>
     <row r="13">
@@ -2454,7 +2454,7 @@
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14" t="n">
-        <v>0.186462845955995</v>
+        <v>0.186952867332309</v>
       </c>
       <c r="F14" t="n">
         <v>47179.08</v>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="H14"/>
       <c r="I14" t="n">
-        <v>-0.729407691489453</v>
+        <v>-0.728267869600161</v>
       </c>
     </row>
   </sheetData>
@@ -2582,7 +2582,7 @@
         <v>0.10472695502504</v>
       </c>
       <c r="E4" t="n">
-        <v>0.227107949809334</v>
+        <v>0.226952277503813</v>
       </c>
       <c r="F4" t="n">
         <v>13985.22</v>
@@ -2594,7 +2594,7 @@
         <v>1.15536069306266</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.643767663235581</v>
+        <v>-0.64406545468198</v>
       </c>
     </row>
     <row r="5">
@@ -2611,7 +2611,7 @@
         <v>0.0768117708525735</v>
       </c>
       <c r="E5" t="n">
-        <v>0.258943438038391</v>
+        <v>0.258582477591671</v>
       </c>
       <c r="F5" t="n">
         <v>10376.8242857143</v>
@@ -2623,7 +2623,7 @@
         <v>1.28496553292348</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.586795090090482</v>
+        <v>-0.587400907696447</v>
       </c>
     </row>
     <row r="6">
@@ -2640,7 +2640,7 @@
         <v>0.0279077813421051</v>
       </c>
       <c r="E6" t="n">
-        <v>0.18522684647642</v>
+        <v>0.185682797933314</v>
       </c>
       <c r="F6" t="n">
         <v>14716.8514285714</v>
@@ -2652,7 +2652,7 @@
         <v>0.832185094445576</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.732296067159545</v>
+        <v>-0.731228328401752</v>
       </c>
     </row>
     <row r="7">
@@ -2694,7 +2694,7 @@
         <v>0.0490018181170012</v>
       </c>
       <c r="E8" t="n">
-        <v>0.346273489592434</v>
+        <v>0.346783836740215</v>
       </c>
       <c r="F8" t="n">
         <v>7578.6</v>
@@ -2706,7 +2706,7 @@
         <v>1.72247100580547</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.460580756398657</v>
+        <v>-0.459941152770569</v>
       </c>
     </row>
     <row r="9">
@@ -2853,7 +2853,7 @@
         <v>0.111120888231963</v>
       </c>
       <c r="E4" t="n">
-        <v>0.237758928017856</v>
+        <v>0.23773763726534</v>
       </c>
       <c r="F4" t="n">
         <v>7865.22</v>
@@ -2865,7 +2865,7 @@
         <v>1.28038038416888</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.623863166015831</v>
+        <v>-0.623902057806076</v>
       </c>
     </row>
     <row r="5">
@@ -2882,7 +2882,7 @@
         <v>0.0463166323010258</v>
       </c>
       <c r="E5" t="n">
-        <v>0.218569566722467</v>
+        <v>0.21568387517109</v>
       </c>
       <c r="F5" t="n">
         <v>11809.8514285714</v>
@@ -2894,7 +2894,7 @@
         <v>1.2287855615693</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.660410308647128</v>
+        <v>-0.666182322148197</v>
       </c>
     </row>
     <row r="6">
@@ -2911,7 +2911,7 @@
         <v>0.0437964783271548</v>
       </c>
       <c r="E6" t="n">
-        <v>0.184070989202584</v>
+        <v>0.184310511172043</v>
       </c>
       <c r="F6" t="n">
         <v>11124.8485714286</v>
@@ -2923,7 +2923,7 @@
         <v>0.652675896147369</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.735014653766717</v>
+        <v>-0.734449896393269</v>
       </c>
     </row>
     <row r="7">
@@ -2969,7 +2969,7 @@
         <v>0.142353917790553</v>
       </c>
       <c r="E8" t="n">
-        <v>0.398722933657988</v>
+        <v>0.398938311717069</v>
       </c>
       <c r="F8" t="n">
         <v>7573.71857142857</v>
@@ -2981,7 +2981,7 @@
         <v>2.02378082367035</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.399328783964715</v>
+        <v>-0.399094254569193</v>
       </c>
     </row>
     <row r="9">
@@ -2998,7 +2998,7 @@
         <v>0.0131382698505472</v>
       </c>
       <c r="E9" t="n">
-        <v>0.110956390662781</v>
+        <v>0.110887957954024</v>
       </c>
       <c r="F9" t="n">
         <v>6248.55642857143</v>
@@ -3010,7 +3010,7 @@
         <v>0.903190308194961</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.95484767901419</v>
+        <v>-0.955115614158115</v>
       </c>
     </row>
     <row r="10">
@@ -3027,7 +3027,7 @@
         <v>0.154867311917387</v>
       </c>
       <c r="E10" t="n">
-        <v>0.327003484688787</v>
+        <v>0.338755228520558</v>
       </c>
       <c r="F10" t="n">
         <v>3951.225</v>
@@ -3039,7 +3039,7 @@
         <v>2.10223824332676</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.48544761928758</v>
+        <v>-0.470113992943802</v>
       </c>
     </row>
   </sheetData>
@@ -3157,7 +3157,7 @@
         <v>0.166262713408938</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.0713653021975958</v>
+        <v>-0.0718485345186965</v>
       </c>
       <c r="F4" t="n">
         <v>4953.66642857143</v>
@@ -3211,7 +3211,7 @@
         <v>0.0375554805809119</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.14320460248576</v>
+        <v>-0.14322728968482</v>
       </c>
       <c r="F6" t="n">
         <v>29225.04</v>
@@ -3240,7 +3240,7 @@
         <v>0.426859527793496</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0430583138148867</v>
+        <v>0.0430076588941056</v>
       </c>
       <c r="F7" t="n">
         <v>2600.08928571429</v>
@@ -3252,7 +3252,7 @@
         <v>2.23822425210174</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.36594298136875</v>
+        <v>-1.36645419746087</v>
       </c>
     </row>
     <row r="8">
@@ -3269,7 +3269,7 @@
         <v>0.131401183260687</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0888937886209107</v>
+        <v>-0.089021967023526</v>
       </c>
       <c r="F8" t="n">
         <v>20644.0714285714</v>
@@ -3298,7 +3298,7 @@
         <v>0.0192449199286524</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0323948686912526</v>
+        <v>0.0322295008782968</v>
       </c>
       <c r="F9" t="n">
         <v>63472.4142857143</v>
@@ -3310,7 +3310,7 @@
         <v>0.197414982211926</v>
       </c>
       <c r="I9" t="n">
-        <v>-1.48952377607612</v>
+        <v>-1.49174642013085</v>
       </c>
     </row>
     <row r="10">
@@ -3327,7 +3327,7 @@
         <v>0.0323205086994282</v>
       </c>
       <c r="E10" t="n">
-        <v>0.146696588771965</v>
+        <v>0.146809310279103</v>
       </c>
       <c r="F10" t="n">
         <v>11464.035</v>
@@ -3339,7 +3339,7 @@
         <v>1.24169249236021</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.833579984962012</v>
+        <v>-0.833246401677268</v>
       </c>
     </row>
     <row r="11">
@@ -3356,7 +3356,7 @@
         <v>0.20143331114612</v>
       </c>
       <c r="E11" t="n">
-        <v>0.102308668556731</v>
+        <v>0.1019830414486</v>
       </c>
       <c r="F11" t="n">
         <v>1878.47571428571</v>
@@ -3368,7 +3368,7 @@
         <v>1.42516441963977</v>
       </c>
       <c r="I11" t="n">
-        <v>-0.990087567198308</v>
+        <v>-0.991472040175493</v>
       </c>
     </row>
     <row r="12">
@@ -3410,7 +3410,7 @@
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13" t="n">
-        <v>0.262243742214757</v>
+        <v>0.262140092531933</v>
       </c>
       <c r="F13" t="n">
         <v>3919.605</v>
@@ -3420,7 +3420,7 @@
       </c>
       <c r="H13"/>
       <c r="I13" t="n">
-        <v>-0.581294866352805</v>
+        <v>-0.581466551606639</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating field day stuff
</commit_message>
<xml_diff>
--- a/04_Output/rC_DG.xlsx
+++ b/04_Output/rC_DG.xlsx
@@ -7,20 +7,21 @@
   </bookViews>
   <sheets>
     <sheet name="13" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="15" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="3" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="5" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="5a" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="6" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="6a" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="7" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="14" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="15" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="5a" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="6" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="6a" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="7" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="9" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
   </si>
   <si>
     <t xml:space="preserve">15</t>
@@ -842,6 +846,387 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>44302</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="n">
+        <v>243.295049119533</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.415059873828465</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.190023104440148</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2055.11785714286</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-165871.125</v>
+      </c>
+      <c r="H2" t="n">
+        <v>2.38613327143824</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-0.721193591042821</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>44386</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1444.94054069675</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.577927133588421</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.835018144430228</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1384.14</v>
+      </c>
+      <c r="G3" t="n">
+        <v>76640.25</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.15984997624233</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-0.0783040874621337</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>44589</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="n">
+        <v>60.5612033684141</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.166262713408938</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.0718485345186965</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4953.66642857143</v>
+      </c>
+      <c r="G4" t="n">
+        <v>953414.764285715</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1.78219449613319</v>
+      </c>
+      <c r="I4" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>44665</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="n">
+        <v>156.869264340194</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0999742912566901</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5" t="n">
+        <v>3506.10428571429</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1052101.76785714</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2.1955378598709</v>
+      </c>
+      <c r="I5"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>44733</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.42172328934366</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0375554805809119</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.14322728968482</v>
+      </c>
+      <c r="F6" t="n">
+        <v>29225.04</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9727288.65000001</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.534244885751498</v>
+      </c>
+      <c r="I6" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>44817</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="n">
+        <v>173.070979705367</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.426859527793496</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0430076588941056</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2600.08928571429</v>
+      </c>
+      <c r="G7" t="n">
+        <v>200400.675000005</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.23822425210174</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-1.36645419746087</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>44879</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="n">
+        <v>16.9540200057436</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.131401183260687</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-0.089021967023526</v>
+      </c>
+      <c r="F8" t="n">
+        <v>20644.0714285714</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3189276.075</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1.22927269128908</v>
+      </c>
+      <c r="I8" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>44953</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.57548757401697</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0192449199286524</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0322295008782968</v>
+      </c>
+      <c r="F9" t="n">
+        <v>63472.4142857143</v>
+      </c>
+      <c r="G9" t="n">
+        <v>64313703.7285714</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.197414982211926</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-1.49174642013085</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>44999</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="n">
+        <v>17.4458643924238</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0323205086994282</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.146809310279103</v>
+      </c>
+      <c r="F10" t="n">
+        <v>11464.035</v>
+      </c>
+      <c r="G10" t="n">
+        <v>11705049.525</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.24169249236021</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-0.833246401677268</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="n">
+        <v>26.617325749677</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.20143331114612</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.1019830414486</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1878.47571428571</v>
+      </c>
+      <c r="G11" t="n">
+        <v>141748.307142857</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.42516441963977</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-0.991472040175493</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>45296</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="n">
+        <v>160.293015632576</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.138009949764872</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.304619300450722</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2495.43</v>
+      </c>
+      <c r="G12" t="n">
+        <v>524364.15</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2.20491459947009</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-0.51624258355513</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>45331</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13" t="n">
+        <v>0.262140092531933</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3919.605</v>
+      </c>
+      <c r="G13" t="n">
+        <v>539592.75</v>
+      </c>
+      <c r="H13"/>
+      <c r="I13" t="n">
+        <v>-0.581466551606639</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
   <dimension ref="A1"/>
@@ -881,32 +1266,28 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44285</v>
+        <v>44292</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>218.653058116812</v>
+        <v>45.7971257985546</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0308372725815327</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.33357194499513</v>
-      </c>
+        <v>0.0462709643091429</v>
+      </c>
+      <c r="E2"/>
       <c r="F2" t="n">
-        <v>5488.14642857143</v>
+        <v>5458.85785714287</v>
       </c>
       <c r="G2" t="n">
-        <v>4876410.9</v>
+        <v>3562871.65714287</v>
       </c>
       <c r="H2" t="n">
-        <v>2.33975555583577</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-0.476810482753012</v>
-      </c>
+        <v>1.6608382227856</v>
+      </c>
+      <c r="I2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -916,54 +1297,54 @@
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>2.06639791095437</v>
+        <v>7.31312382905134</v>
       </c>
       <c r="D3" t="n">
-        <v>0.028469917352607</v>
+        <v>0.0186472739593504</v>
       </c>
       <c r="E3" t="n">
-        <v>0.103246752096473</v>
+        <v>0.47962197581167</v>
       </c>
       <c r="F3" t="n">
-        <v>24196.695</v>
+        <v>13674.0471428571</v>
       </c>
       <c r="G3" t="n">
-        <v>9603914.55</v>
+        <v>7186340.60357143</v>
       </c>
       <c r="H3" t="n">
-        <v>0.315213954111133</v>
+        <v>0.864102927153004</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.986123601354522</v>
+        <v>-0.319100926167242</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44510</v>
+        <v>44517</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>56.4532973967771</v>
+        <v>22.5234747698149</v>
       </c>
       <c r="D4" t="n">
-        <v>0.230530622192957</v>
+        <v>0.026820127000421</v>
       </c>
       <c r="E4" t="n">
-        <v>0.208368019852923</v>
+        <v>0.52571156242498</v>
       </c>
       <c r="F4" t="n">
-        <v>7971.19071428572</v>
+        <v>11099.5307142857</v>
       </c>
       <c r="G4" t="n">
-        <v>926679.107142858</v>
+        <v>11091201.1392857</v>
       </c>
       <c r="H4" t="n">
-        <v>1.75168931383232</v>
+        <v>1.35263539137228</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.681168935406929</v>
+        <v>-0.279252471065758</v>
       </c>
     </row>
     <row r="5">
@@ -974,137 +1355,137 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>4.20435343981279</v>
+        <v>13.3793659977175</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0173910258844274</v>
+        <v>0.0205672011357402</v>
       </c>
       <c r="E5" t="n">
-        <v>0.115660292693498</v>
+        <v>0.537089994272753</v>
       </c>
       <c r="F5" t="n">
-        <v>11892.435</v>
+        <v>3737.09785714286</v>
       </c>
       <c r="G5" t="n">
-        <v>9368415.675</v>
+        <v>1835188.37142857</v>
       </c>
       <c r="H5" t="n">
-        <v>0.623699217943341</v>
+        <v>1.1264355341929</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.936815712992044</v>
+        <v>-0.269952938245627</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44659</v>
+        <v>44666</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>45.7221685893927</v>
+        <v>8.55028667889765</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0816494874119976</v>
+        <v>0.0127442482204935</v>
       </c>
       <c r="E6"/>
       <c r="F6" t="n">
-        <v>6561.36857142857</v>
+        <v>17543.2714285714</v>
       </c>
       <c r="G6" t="n">
-        <v>1149150.76071429</v>
+        <v>11838449.1321429</v>
       </c>
       <c r="H6" t="n">
-        <v>1.66012682067494</v>
+        <v>0.931980676245845</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44733</v>
+        <v>44818</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>5.84854833181856</v>
+        <v>80.2971338081475</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0217811972641943</v>
+        <v>0.0756138674831853</v>
       </c>
       <c r="E7" t="n">
-        <v>0.118618295568362</v>
+        <v>0.733067126241204</v>
       </c>
       <c r="F7" t="n">
-        <v>8549.13</v>
+        <v>4981.49785714286</v>
       </c>
       <c r="G7" t="n">
-        <v>3925004.625</v>
+        <v>1686547.05</v>
       </c>
       <c r="H7" t="n">
-        <v>0.767048083224665</v>
+        <v>1.90470004349137</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.925848320654844</v>
+        <v>-0.134856255616212</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44806</v>
+        <v>44998</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="n">
-        <v>94.0961393698247</v>
+        <v>73.3277604235412</v>
       </c>
       <c r="D8" t="n">
-        <v>0.125964440018116</v>
+        <v>0.0601797177022106</v>
       </c>
       <c r="E8" t="n">
-        <v>0.32669127366084</v>
+        <v>0.604935952376543</v>
       </c>
       <c r="F8" t="n">
-        <v>6376.45714285715</v>
+        <v>6818.7</v>
       </c>
       <c r="G8" t="n">
-        <v>1543943.21785715</v>
+        <v>2266112.325</v>
       </c>
       <c r="H8" t="n">
-        <v>1.97357180531061</v>
+        <v>1.8652684209761</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.485862465927253</v>
+        <v>-0.218290603863035</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44998</v>
+        <v>45140</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>4.110400422878</v>
+        <v>203.61423579318</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0135347353218176</v>
+        <v>0.151213418262108</v>
       </c>
       <c r="E9" t="n">
-        <v>0.148399542142312</v>
+        <v>0.861815715904159</v>
       </c>
       <c r="F9" t="n">
-        <v>121642.65</v>
+        <v>6875.74714285714</v>
       </c>
       <c r="G9" t="n">
-        <v>139305352.5</v>
+        <v>682057.242857143</v>
       </c>
       <c r="H9" t="n">
-        <v>0.61388413160249</v>
+        <v>2.30880813864651</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.828567438985388</v>
+        <v>-0.0645855904655424</v>
       </c>
     </row>
     <row r="10">
@@ -1115,25 +1496,25 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>850.231688135016</v>
+        <v>587.941323455919</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.264707017120813</v>
+        <v>0.116204075358259</v>
       </c>
       <c r="E10" t="n">
-        <v>0.528260069853473</v>
+        <v>1.08829296279805</v>
       </c>
       <c r="F10" t="n">
-        <v>1999.455</v>
+        <v>2041.02</v>
       </c>
       <c r="G10" t="n">
-        <v>-105748.499999999</v>
+        <v>298589.7</v>
       </c>
       <c r="H10" t="n">
-        <v>2.92953728708808</v>
+        <v>2.7693339856495</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.277152215543772</v>
+        <v>0.0367458209135808</v>
       </c>
     </row>
   </sheetData>
@@ -1181,201 +1562,259 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44299</v>
+        <v>44285</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>201.556447682785</v>
+        <v>218.653058116812</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0966260418499097</v>
+        <v>0.0308372725815327</v>
       </c>
       <c r="E2" t="n">
-        <v>0.550747337517402</v>
+        <v>0.33357194499513</v>
       </c>
       <c r="F2" t="n">
-        <v>1984.55571428571</v>
+        <v>5488.14642857143</v>
       </c>
       <c r="G2" t="n">
-        <v>626424.803571428</v>
+        <v>4876410.9</v>
       </c>
       <c r="H2" t="n">
-        <v>2.30439669555911</v>
+        <v>2.33975555583577</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.259047593685675</v>
+        <v>-0.476810482753012</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44371</v>
+        <v>44452</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>416.243786340365</v>
+        <v>2.06639791095437</v>
       </c>
       <c r="D3" t="n">
-        <v>0.214345900534267</v>
+        <v>0.028469917352607</v>
       </c>
       <c r="E3" t="n">
-        <v>0.89859430101436</v>
+        <v>0.103246752096473</v>
       </c>
       <c r="F3" t="n">
-        <v>3363.41357142857</v>
+        <v>24196.695</v>
       </c>
       <c r="G3" t="n">
-        <v>643352.432142857</v>
+        <v>9603914.55</v>
       </c>
       <c r="H3" t="n">
-        <v>2.61934776344354</v>
+        <v>0.315213954111133</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0464363400784758</v>
+        <v>-0.986123601354522</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44452</v>
+        <v>44510</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>41.9734413050142</v>
+        <v>56.4532973967771</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0482196240014123</v>
+        <v>0.230530622192957</v>
       </c>
       <c r="E4" t="n">
-        <v>0.506400216436797</v>
+        <v>0.208368019852923</v>
       </c>
       <c r="F4" t="n">
-        <v>14294.7535714286</v>
+        <v>7971.19071428572</v>
       </c>
       <c r="G4" t="n">
-        <v>4980376.03928571</v>
+        <v>926679.107142858</v>
       </c>
       <c r="H4" t="n">
-        <v>1.62297457746762</v>
+        <v>1.75168931383232</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.295506117372047</v>
+        <v>-0.681168935406929</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44517</v>
+        <v>44589</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="n">
-        <v>61.6453450829362</v>
+        <v>4.20435343981279</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0396467471682954</v>
+        <v>0.0173910258844274</v>
       </c>
       <c r="E5" t="n">
-        <v>0.542257562907983</v>
+        <v>0.115660292693498</v>
       </c>
       <c r="F5" t="n">
-        <v>9733.09499999999</v>
+        <v>11892.435</v>
       </c>
       <c r="G5" t="n">
-        <v>7413961.79999999</v>
+        <v>9368415.675</v>
       </c>
       <c r="H5" t="n">
-        <v>1.78990028805065</v>
+        <v>0.623699217943341</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.26579438213295</v>
+        <v>-0.936815712992044</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44589</v>
+        <v>44659</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>18.3696008298861</v>
+        <v>45.7221685893927</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0240540549037401</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.47259266099701</v>
-      </c>
+        <v>0.0816494874119976</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="n">
-        <v>5443.77642857143</v>
+        <v>6561.36857142857</v>
       </c>
       <c r="G6" t="n">
-        <v>2896822.95</v>
+        <v>1149150.76071429</v>
       </c>
       <c r="H6" t="n">
-        <v>1.26409971922027</v>
-      </c>
-      <c r="I6" t="n">
-        <v>-0.32551302691281</v>
-      </c>
+        <v>1.66012682067494</v>
+      </c>
+      <c r="I6"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44666</v>
+        <v>44733</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>43.1380098171326</v>
+        <v>5.84854833181856</v>
       </c>
       <c r="D7" t="n">
-        <v>0.026222037675287</v>
-      </c>
-      <c r="E7"/>
+        <v>0.0217811972641943</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.118618295568362</v>
+      </c>
       <c r="F7" t="n">
-        <v>9272.565</v>
+        <v>8549.13</v>
       </c>
       <c r="G7" t="n">
-        <v>14109328.5</v>
+        <v>3925004.625</v>
       </c>
       <c r="H7" t="n">
-        <v>1.63486010494421</v>
-      </c>
-      <c r="I7"/>
+        <v>0.767048083224665</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.925848320654844</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44818</v>
+        <v>44806</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>268.141444612033</v>
+        <v>94.0961393698247</v>
       </c>
       <c r="D8" t="n">
-        <v>0.117343468865951</v>
+        <v>0.125964440018116</v>
       </c>
       <c r="E8" t="n">
-        <v>0.837560505687049</v>
+        <v>0.32669127366084</v>
       </c>
       <c r="F8" t="n">
-        <v>2237.625</v>
+        <v>6376.45714285715</v>
       </c>
       <c r="G8" t="n">
-        <v>444308.174999999</v>
+        <v>1543943.21785715</v>
       </c>
       <c r="H8" t="n">
-        <v>2.42836394481183</v>
+        <v>1.97357180531061</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.0769838095605552</v>
+        <v>-0.485862465927253</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>44998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.110400422878</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0135347353218176</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.148399542142312</v>
+      </c>
+      <c r="F9" t="n">
+        <v>121642.65</v>
+      </c>
+      <c r="G9" t="n">
+        <v>139305352.5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.61388413160249</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-0.828567438985388</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>45279</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="n">
+        <v>850.231688135016</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.264707017120813</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.528260069853473</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1999.455</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-105748.499999999</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.92953728708808</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-0.277152215543772</v>
       </c>
     </row>
   </sheetData>
@@ -1423,346 +1862,201 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44386</v>
+        <v>44299</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>1661.73191635079</v>
+        <v>201.556447682785</v>
       </c>
       <c r="D2" t="n">
-        <v>0.387436294953374</v>
+        <v>0.0966260418499097</v>
       </c>
       <c r="E2" t="n">
-        <v>0.843910837480766</v>
+        <v>0.550747337517402</v>
       </c>
       <c r="F2" t="n">
-        <v>1203.56357142857</v>
+        <v>1984.55571428571</v>
       </c>
       <c r="G2" t="n">
-        <v>178933.317857143</v>
+        <v>626424.803571428</v>
       </c>
       <c r="H2" t="n">
-        <v>3.22056096130097</v>
+        <v>2.30439669555911</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.0737034358810179</v>
+        <v>-0.259047593685675</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44452</v>
+        <v>44371</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="n">
-        <v>25.6084522525835</v>
+        <v>416.243786340365</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0748083206536477</v>
+        <v>0.214345900534267</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0314608700934574</v>
+        <v>0.89859430101436</v>
       </c>
       <c r="F3" t="n">
-        <v>11714.8821428571</v>
+        <v>3363.41357142857</v>
       </c>
       <c r="G3" t="n">
-        <v>3774027.50357143</v>
+        <v>643352.432142857</v>
       </c>
       <c r="H3" t="n">
-        <v>1.40838333096844</v>
+        <v>2.61934776344354</v>
       </c>
       <c r="I3" t="n">
-        <v>-1.50222927053785</v>
+        <v>-0.0464363400784758</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44510</v>
+        <v>44452</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>326.494767171751</v>
+        <v>41.9734413050142</v>
       </c>
       <c r="D4" t="n">
-        <v>0.181034619271933</v>
+        <v>0.0482196240014123</v>
       </c>
       <c r="E4" t="n">
-        <v>0.298854491442191</v>
+        <v>0.506400216436797</v>
       </c>
       <c r="F4" t="n">
-        <v>4287.97071428572</v>
+        <v>14294.7535714286</v>
       </c>
       <c r="G4" t="n">
-        <v>959279.58214286</v>
+        <v>4980376.03928571</v>
       </c>
       <c r="H4" t="n">
-        <v>2.51387622510069</v>
+        <v>1.62297457746762</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.524540212830461</v>
+        <v>-0.295506117372047</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44589</v>
+        <v>44517</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="n">
-        <v>55.2594896825599</v>
+        <v>61.6453450829362</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0466003004043193</v>
+        <v>0.0396467471682954</v>
       </c>
       <c r="E5" t="n">
-        <v>0.071022433807391</v>
+        <v>0.542257562907983</v>
       </c>
       <c r="F5" t="n">
-        <v>3619.28785714286</v>
+        <v>9733.09499999999</v>
       </c>
       <c r="G5" t="n">
-        <v>1654299.02142857</v>
+        <v>7413961.79999999</v>
       </c>
       <c r="H5" t="n">
-        <v>1.74240686992049</v>
+        <v>1.78990028805065</v>
       </c>
       <c r="I5" t="n">
-        <v>-1.1486044493111</v>
+        <v>-0.26579438213295</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44659</v>
+        <v>44589</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="n">
-        <v>-59.2075325514556</v>
+        <v>18.3696008298861</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00694043951640586</v>
-      </c>
-      <c r="E6"/>
+        <v>0.0240540549037401</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.47259266099701</v>
+      </c>
       <c r="F6" t="n">
-        <v>-20267.6914285714</v>
+        <v>5443.77642857143</v>
       </c>
       <c r="G6" t="n">
-        <v>-90527182.4357143</v>
-      </c>
-      <c r="H6" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="I6"/>
+        <v>2896822.95</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1.26409971922027</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-0.32551302691281</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44733</v>
+        <v>44666</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>19.3061500671871</v>
+        <v>43.1380098171326</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0247248402753767</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.00408688713481306</v>
-      </c>
+        <v>0.026222037675287</v>
+      </c>
+      <c r="E7"/>
       <c r="F7" t="n">
-        <v>20718.7864285714</v>
+        <v>9272.565</v>
       </c>
       <c r="G7" t="n">
-        <v>24301261.3928571</v>
+        <v>14109328.5</v>
       </c>
       <c r="H7" t="n">
-        <v>1.28569567764907</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-2.38860735578112</v>
-      </c>
+        <v>1.63486010494421</v>
+      </c>
+      <c r="I7"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44806</v>
+        <v>44818</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="n">
-        <v>83.4160791046595</v>
+        <v>268.141444612033</v>
       </c>
       <c r="D8" t="n">
-        <v>0.104270024651914</v>
+        <v>0.117343468865951</v>
       </c>
       <c r="E8" t="n">
-        <v>0.292886326762752</v>
+        <v>0.837560505687049</v>
       </c>
       <c r="F8" t="n">
-        <v>11988.0964285714</v>
+        <v>2237.625</v>
       </c>
       <c r="G8" t="n">
-        <v>4242453.76071428</v>
+        <v>444308.174999999</v>
       </c>
       <c r="H8" t="n">
-        <v>1.92124977238071</v>
+        <v>2.42836394481183</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.533300902644435</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>44879</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="n">
-        <v>62.1041048151678</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0.0624314324451668</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.100958463791928</v>
-      </c>
-      <c r="F9" t="n">
-        <v>7245.89785714286</v>
-      </c>
-      <c r="G9" t="n">
-        <v>3017604.06428571</v>
-      </c>
-      <c r="H9" t="n">
-        <v>1.79312030612925</v>
-      </c>
-      <c r="I9" t="n">
-        <v>-0.995857266378117</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>44959</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="n">
-        <v>30.1205661719794</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.017179789481342</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.100905322589866</v>
-      </c>
-      <c r="F10" t="n">
-        <v>6639.98142857143</v>
-      </c>
-      <c r="G10" t="n">
-        <v>10435488.675</v>
-      </c>
-      <c r="H10" t="n">
-        <v>1.47886313097672</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-0.996085924838993</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>44999</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="n">
-        <v>203.383280877396</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.223866557705922</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.292268158933349</v>
-      </c>
-      <c r="F11" t="n">
-        <v>2950.095</v>
-      </c>
-      <c r="G11" t="n">
-        <v>466498.274999997</v>
-      </c>
-      <c r="H11" t="n">
-        <v>2.30831524887617</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-0.534218496147122</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>45047</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="n">
-        <v>7.12054440834328</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.0106085660132641</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.0398067631956158</v>
-      </c>
-      <c r="F12" t="n">
-        <v>7021.935</v>
-      </c>
-      <c r="G12" t="n">
-        <v>16680177.3</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.852513199325168</v>
-      </c>
-      <c r="I12" t="n">
-        <v>-1.40004313473525</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>45279</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="n">
-        <v>1159.08432338453</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.192383869915185</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.69658739105357</v>
-      </c>
-      <c r="F13" t="n">
-        <v>3105.9</v>
-      </c>
-      <c r="G13" t="n">
-        <v>613482.825</v>
-      </c>
-      <c r="H13" t="n">
-        <v>3.06411503203648</v>
-      </c>
-      <c r="I13" t="n">
-        <v>-0.157024390982315</v>
+        <v>-0.0769838095605552</v>
       </c>
     </row>
   </sheetData>
@@ -1810,164 +2104,172 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44299</v>
+        <v>44386</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>23.3064027849153</v>
+        <v>1661.73191635079</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0288993102026876</v>
-      </c>
-      <c r="E2"/>
+        <v>0.387436294953374</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.843910837480766</v>
+      </c>
       <c r="F2" t="n">
-        <v>4290.66642857143</v>
+        <v>1203.56357142857</v>
       </c>
       <c r="G2" t="n">
-        <v>2672451.18214286</v>
+        <v>178933.317857143</v>
       </c>
       <c r="H2" t="n">
-        <v>1.36747524772831</v>
-      </c>
-      <c r="I2"/>
+        <v>3.22056096130097</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-0.0737034358810179</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44386</v>
+        <v>44452</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>270.901397309407</v>
+        <v>25.6084522525835</v>
       </c>
       <c r="D3" t="n">
-        <v>0.233297132170326</v>
-      </c>
-      <c r="E3"/>
+        <v>0.0748083206536477</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.0314608700934574</v>
+      </c>
       <c r="F3" t="n">
-        <v>3691.38</v>
+        <v>11714.8821428571</v>
       </c>
       <c r="G3" t="n">
-        <v>424047.15</v>
+        <v>3774027.50357143</v>
       </c>
       <c r="H3" t="n">
-        <v>2.43281124512988</v>
-      </c>
-      <c r="I3"/>
+        <v>1.40838333096844</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-1.50222927053785</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44452</v>
+        <v>44510</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="n">
-        <v>2.04807802379181</v>
+        <v>326.494767171751</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0334046106509795</v>
+        <v>0.181034619271933</v>
       </c>
       <c r="E4" t="n">
-        <v>0.47844128219725</v>
+        <v>0.298854491442191</v>
       </c>
       <c r="F4" t="n">
-        <v>24413.1324193548</v>
+        <v>4287.97071428572</v>
       </c>
       <c r="G4" t="n">
-        <v>4019571.72048387</v>
+        <v>959279.58214286</v>
       </c>
       <c r="H4" t="n">
-        <v>0.311346497546363</v>
+        <v>2.51387622510069</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.320171354402254</v>
+        <v>-0.524540212830461</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44510</v>
+        <v>44589</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>21.1919407049499</v>
+        <v>55.2594896825599</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0277510769684758</v>
-      </c>
-      <c r="E5"/>
+        <v>0.0466003004043193</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.071022433807391</v>
+      </c>
       <c r="F5" t="n">
-        <v>9437.55</v>
+        <v>3619.28785714286</v>
       </c>
       <c r="G5" t="n">
-        <v>5271219.75</v>
+        <v>1654299.02142857</v>
       </c>
       <c r="H5" t="n">
-        <v>1.32617073013491</v>
-      </c>
-      <c r="I5"/>
+        <v>1.74240686992049</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-1.1486044493111</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44589</v>
+        <v>44659</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="n">
-        <v>138.347849975591</v>
+        <v>-59.2075325514556</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00958213989251452</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.455538766986625</v>
-      </c>
+        <v>0.00694043951640586</v>
+      </c>
+      <c r="E6"/>
       <c r="F6" t="n">
-        <v>722.815714285718</v>
+        <v>-20267.6914285714</v>
       </c>
       <c r="G6" t="n">
-        <v>618555.867857144</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2.14097241428295</v>
-      </c>
-      <c r="I6" t="n">
-        <v>-0.341474658050028</v>
-      </c>
+        <v>-90527182.4357143</v>
+      </c>
+      <c r="H6" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="I6"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44659</v>
+        <v>44733</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>10.1562152863735</v>
+        <v>19.3061500671871</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0160991553702436</v>
+        <v>0.0247248402753767</v>
       </c>
       <c r="E7" t="n">
-        <v>0.554639976552681</v>
+        <v>0.00408688713481306</v>
       </c>
       <c r="F7" t="n">
-        <v>19692.375</v>
+        <v>20718.7864285714</v>
       </c>
       <c r="G7" t="n">
-        <v>12231930.525</v>
+        <v>24301261.3928571</v>
       </c>
       <c r="H7" t="n">
-        <v>1.00673189825654</v>
+        <v>1.28569567764907</v>
       </c>
       <c r="I7" t="n">
-        <v>-0.255988831169016</v>
+        <v>-2.38860735578112</v>
       </c>
     </row>
     <row r="8">
@@ -1978,83 +2280,170 @@
         <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>35.2877784497159</v>
+        <v>83.4160791046595</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0598939505762173</v>
+        <v>0.104270024651914</v>
       </c>
       <c r="E8" t="n">
-        <v>0.578629035198701</v>
+        <v>0.292886326762752</v>
       </c>
       <c r="F8" t="n">
-        <v>22670.7385714286</v>
+        <v>11988.0964285714</v>
       </c>
       <c r="G8" t="n">
-        <v>9576420.99642858</v>
+        <v>4242453.76071428</v>
       </c>
       <c r="H8" t="n">
-        <v>1.54762431811064</v>
+        <v>1.92124977238071</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.237599777549088</v>
+        <v>-0.533300902644435</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45140</v>
+        <v>44879</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
       <c r="C9" t="n">
-        <v>139.040343548826</v>
+        <v>62.1041048151678</v>
       </c>
       <c r="D9" t="n">
-        <v>0.114325713526605</v>
+        <v>0.0624314324451668</v>
       </c>
       <c r="E9" t="n">
-        <v>0.603687349344395</v>
+        <v>0.100958463791928</v>
       </c>
       <c r="F9" t="n">
-        <v>6113.33357142857</v>
+        <v>7245.89785714286</v>
       </c>
       <c r="G9" t="n">
-        <v>962513.164285714</v>
+        <v>3017604.06428571</v>
       </c>
       <c r="H9" t="n">
-        <v>2.14314083218554</v>
+        <v>1.79312030612925</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.219187924970591</v>
+        <v>-0.995857266378117</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45197</v>
+        <v>44959</v>
       </c>
       <c r="B10" t="s">
         <v>13</v>
       </c>
       <c r="C10" t="n">
-        <v>18.5478970626159</v>
+        <v>30.1205661719794</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0380123901994629</v>
+        <v>0.017179789481342</v>
       </c>
       <c r="E10" t="n">
-        <v>0.46420761962736</v>
+        <v>0.100905322589866</v>
       </c>
       <c r="F10" t="n">
-        <v>10782.8935714286</v>
+        <v>6639.98142857143</v>
       </c>
       <c r="G10" t="n">
-        <v>5673357.30000001</v>
+        <v>10435488.675</v>
       </c>
       <c r="H10" t="n">
-        <v>1.26829467697673</v>
+        <v>1.47886313097672</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.333287735196435</v>
+        <v>-0.996085924838993</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>44999</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="n">
+        <v>203.383280877396</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.223866557705922</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.292268158933349</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2950.095</v>
+      </c>
+      <c r="G11" t="n">
+        <v>466498.274999997</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2.30831524887617</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-0.534218496147122</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>45047</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="n">
+        <v>7.12054440834328</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0106085660132641</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0398067631956158</v>
+      </c>
+      <c r="F12" t="n">
+        <v>7021.935</v>
+      </c>
+      <c r="G12" t="n">
+        <v>16680177.3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.852513199325168</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-1.40004313473525</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>45279</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1159.08432338453</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.192383869915185</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.69658739105357</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3105.9</v>
+      </c>
+      <c r="G13" t="n">
+        <v>613482.825</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3.06411503203648</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-0.157024390982315</v>
       </c>
     </row>
   </sheetData>
@@ -2102,369 +2491,251 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44292</v>
+        <v>44299</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>1474.27392009435</v>
+        <v>23.3064027849153</v>
       </c>
       <c r="D2" t="n">
-        <v>0.609595398242257</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.642692214475338</v>
-      </c>
+        <v>0.0288993102026876</v>
+      </c>
+      <c r="E2"/>
       <c r="F2" t="n">
-        <v>1356.6</v>
+        <v>4290.66642857143</v>
       </c>
       <c r="G2" t="n">
-        <v>111270.525</v>
+        <v>2672451.18214286</v>
       </c>
       <c r="H2" t="n">
-        <v>3.16857818293498</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-0.191996961068096</v>
-      </c>
+        <v>1.36747524772831</v>
+      </c>
+      <c r="I2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44452</v>
+        <v>44386</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>163.514515592335</v>
+        <v>270.901397309407</v>
       </c>
       <c r="D3" t="n">
-        <v>0.19909322659857</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.456824240921209</v>
-      </c>
+        <v>0.233297132170326</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" t="n">
-        <v>6115.665</v>
+        <v>3691.38</v>
       </c>
       <c r="G3" t="n">
-        <v>1170340.35</v>
+        <v>424047.15</v>
       </c>
       <c r="H3" t="n">
-        <v>2.21355631211454</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-0.340250858748654</v>
-      </c>
+        <v>2.43281124512988</v>
+      </c>
+      <c r="I3"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44589</v>
+        <v>44452</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>65.6511558308027</v>
+        <v>2.04807802379181</v>
       </c>
       <c r="D4" t="n">
-        <v>0.09276270132275</v>
+        <v>0.0334046106509795</v>
       </c>
       <c r="E4" t="n">
-        <v>0.38887615975603</v>
+        <v>0.47844128219725</v>
       </c>
       <c r="F4" t="n">
-        <v>7616.01214285714</v>
+        <v>24413.1324193548</v>
       </c>
       <c r="G4" t="n">
-        <v>2101813.63928571</v>
+        <v>4019571.72048387</v>
       </c>
       <c r="H4" t="n">
-        <v>1.81724237652635</v>
+        <v>0.311346497546363</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.410188680672972</v>
+        <v>-0.320171354402254</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44665</v>
+        <v>44510</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
       </c>
       <c r="C5" t="n">
-        <v>33.6536236839781</v>
+        <v>21.1919407049499</v>
       </c>
       <c r="D5" t="n">
-        <v>0.132219643097552</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.317914439292082</v>
-      </c>
+        <v>0.0277510769684758</v>
+      </c>
+      <c r="E5"/>
       <c r="F5" t="n">
-        <v>17828.6892857143</v>
+        <v>9437.55</v>
       </c>
       <c r="G5" t="n">
-        <v>3640719.33214286</v>
+        <v>5271219.75</v>
       </c>
       <c r="H5" t="n">
-        <v>1.5270318341239</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-0.497689746503399</v>
-      </c>
+        <v>1.32617073013491</v>
+      </c>
+      <c r="I5"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44817</v>
+        <v>44589</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6" t="n">
-        <v>1147.67621184873</v>
+        <v>138.347849975591</v>
       </c>
       <c r="D6" t="n">
-        <v>0.370207050897618</v>
+        <v>0.00958213989251452</v>
       </c>
       <c r="E6" t="n">
-        <v>0.810515482511753</v>
+        <v>0.455538766986625</v>
       </c>
       <c r="F6" t="n">
-        <v>1394.12142857143</v>
+        <v>722.815714285718</v>
       </c>
       <c r="G6" t="n">
-        <v>158539.692857143</v>
+        <v>618555.867857144</v>
       </c>
       <c r="H6" t="n">
-        <v>3.05981938001173</v>
+        <v>2.14097241428295</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.0912386848189221</v>
+        <v>-0.341474658050028</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44880</v>
+        <v>44659</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7" t="n">
-        <v>20.7914719322554</v>
+        <v>10.1562152863735</v>
       </c>
       <c r="D7" t="n">
-        <v>0.108285591446864</v>
-      </c>
-      <c r="E7"/>
+        <v>0.0160991553702436</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.554639976552681</v>
+      </c>
       <c r="F7" t="n">
-        <v>9619.32857142857</v>
+        <v>19692.375</v>
       </c>
       <c r="G7" t="n">
-        <v>1687826.05714286</v>
+        <v>12231930.525</v>
       </c>
       <c r="H7" t="n">
-        <v>1.31788523629769</v>
-      </c>
-      <c r="I7"/>
+        <v>1.00673189825654</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-0.255988831169016</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44953</v>
+        <v>44806</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="n">
-        <v>5.13894891976541</v>
+        <v>35.2877784497159</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0176083819768147</v>
+        <v>0.0598939505762173</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0509851313580177</v>
+        <v>0.578629035198701</v>
       </c>
       <c r="F8" t="n">
-        <v>19459.2321428571</v>
+        <v>22670.7385714286</v>
       </c>
       <c r="G8" t="n">
-        <v>27627797.0464286</v>
+        <v>9576420.99642858</v>
       </c>
       <c r="H8" t="n">
-        <v>0.710874300897029</v>
-      </c>
-      <c r="I8" t="e">
-        <v>#NUM!</v>
+        <v>1.54762431811064</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-0.237599777549088</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44998</v>
+        <v>45140</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9" t="n">
-        <v>33.1790704053949</v>
+        <v>139.040343548826</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0942639400766061</v>
+        <v>0.114325713526605</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0410550448373626</v>
+        <v>0.603687349344395</v>
       </c>
       <c r="F9" t="n">
-        <v>18083.6892857143</v>
+        <v>6113.33357142857</v>
       </c>
       <c r="G9" t="n">
-        <v>4604184.19285714</v>
+        <v>962513.164285714</v>
       </c>
       <c r="H9" t="n">
-        <v>1.52086421401315</v>
+        <v>2.14314083218554</v>
       </c>
       <c r="I9" t="n">
-        <v>-1.38663346922879</v>
+        <v>-0.219187924970591</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45140</v>
+        <v>45197</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="n">
-        <v>657.928746316773</v>
+        <v>18.5478970626159</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.624858780565361</v>
+        <v>0.0380123901994629</v>
       </c>
       <c r="E10" t="n">
-        <v>0.489625120007815</v>
+        <v>0.46420761962736</v>
       </c>
       <c r="F10" t="n">
-        <v>1823.90571428572</v>
+        <v>10782.8935714286</v>
       </c>
       <c r="G10" t="n">
-        <v>-61297.0821428564</v>
+        <v>5673357.30000001</v>
       </c>
       <c r="H10" t="n">
-        <v>2.81817886206828</v>
+        <v>1.26829467697673</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.310136308997868</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>45197</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="n">
-        <v>133.328381136318</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.0966021881464723</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.190986898896875</v>
-      </c>
-      <c r="F11" t="n">
-        <v>750.027857142865</v>
-      </c>
-      <c r="G11" t="n">
-        <v>273295.885714292</v>
-      </c>
-      <c r="H11" t="n">
-        <v>2.12492260596996</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-0.718996422971846</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>45231</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="n">
-        <v>17.3551452799212</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.0456410932698102</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.0829762877707573</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2880.99</v>
-      </c>
-      <c r="G12" t="n">
-        <v>1527569.85</v>
-      </c>
-      <c r="H12" t="n">
-        <v>1.23942825350176</v>
-      </c>
-      <c r="I12" t="n">
-        <v>-1.08104599872781</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>45296</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" t="n">
-        <v>236.595392304735</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.229962718506469</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.287726779544469</v>
-      </c>
-      <c r="F13" t="n">
-        <v>2535.975</v>
-      </c>
-      <c r="G13" t="n">
-        <v>628582.649999999</v>
-      </c>
-      <c r="H13" t="n">
-        <v>2.37400628248923</v>
-      </c>
-      <c r="I13" t="n">
-        <v>-0.541019715213791</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>45331</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14"/>
-      <c r="D14"/>
-      <c r="E14" t="n">
-        <v>0.186952867332309</v>
-      </c>
-      <c r="F14" t="n">
-        <v>47179.08</v>
-      </c>
-      <c r="G14" t="n">
-        <v>17329386.9</v>
-      </c>
-      <c r="H14"/>
-      <c r="I14" t="n">
-        <v>-0.728267869600161</v>
+        <v>-0.333287735196435</v>
       </c>
     </row>
   </sheetData>
@@ -2518,224 +2789,363 @@
         <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>79.9725579879591</v>
+        <v>1474.27392009435</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0836415522456026</v>
+        <v>0.609595398242257</v>
       </c>
       <c r="E2" t="n">
-        <v>0.175235931608227</v>
+        <v>0.642692214475338</v>
       </c>
       <c r="F2" t="n">
-        <v>2500.85785714285</v>
+        <v>1356.6</v>
       </c>
       <c r="G2" t="n">
-        <v>774402.396428567</v>
+        <v>111270.525</v>
       </c>
       <c r="H2" t="n">
-        <v>1.90294098750518</v>
+        <v>3.16857818293498</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.756376838240995</v>
+        <v>-0.191996961068096</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44371</v>
+        <v>44452</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" t="n">
-        <v>97.517092917943</v>
+        <v>163.514515592335</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0844166976160872</v>
+        <v>0.19909322659857</v>
       </c>
       <c r="E3" t="n">
-        <v>0.428172659072591</v>
+        <v>0.456824240921209</v>
       </c>
       <c r="F3" t="n">
-        <v>12305.535</v>
+        <v>6115.665</v>
       </c>
       <c r="G3" t="n">
-        <v>5685082.2</v>
+        <v>1170340.35</v>
       </c>
       <c r="H3" t="n">
-        <v>1.9890807460505</v>
+        <v>2.21355631211454</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.368381067992078</v>
+        <v>-0.340250858748654</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44452</v>
+        <v>44589</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>14.3008118570891</v>
+        <v>65.6511558308027</v>
       </c>
       <c r="D4" t="n">
-        <v>0.10472695502504</v>
+        <v>0.09276270132275</v>
       </c>
       <c r="E4" t="n">
-        <v>0.226952277503813</v>
+        <v>0.38887615975603</v>
       </c>
       <c r="F4" t="n">
-        <v>13985.22</v>
+        <v>7616.01214285714</v>
       </c>
       <c r="G4" t="n">
-        <v>1949681.55</v>
+        <v>2101813.63928571</v>
       </c>
       <c r="H4" t="n">
-        <v>1.15536069306266</v>
+        <v>1.81724237652635</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.64406545468198</v>
+        <v>-0.410188680672972</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44517</v>
+        <v>44665</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="n">
-        <v>19.273719443755</v>
+        <v>33.6536236839781</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0768117708525735</v>
+        <v>0.132219643097552</v>
       </c>
       <c r="E5" t="n">
-        <v>0.258582477591671</v>
+        <v>0.317914439292082</v>
       </c>
       <c r="F5" t="n">
-        <v>10376.8242857143</v>
+        <v>17828.6892857143</v>
       </c>
       <c r="G5" t="n">
-        <v>2877506.33571429</v>
+        <v>3640719.33214286</v>
       </c>
       <c r="H5" t="n">
-        <v>1.28496553292348</v>
+        <v>1.5270318341239</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.587400907696447</v>
+        <v>-0.497689746503399</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44589</v>
+        <v>44817</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>6.79493167987407</v>
+        <v>1147.67621184873</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0279077813421051</v>
+        <v>0.370207050897618</v>
       </c>
       <c r="E6" t="n">
-        <v>0.185682797933314</v>
+        <v>0.810515482511753</v>
       </c>
       <c r="F6" t="n">
-        <v>14716.8514285714</v>
+        <v>1394.12142857143</v>
       </c>
       <c r="G6" t="n">
-        <v>4798781.61428571</v>
+        <v>158539.692857143</v>
       </c>
       <c r="H6" t="n">
-        <v>0.832185094445576</v>
+        <v>3.05981938001173</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.731228328401752</v>
+        <v>-0.0912386848189221</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44665</v>
+        <v>44880</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>5.52548180523963</v>
+        <v>20.7914719322554</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0835954778785003</v>
+        <v>0.108285591446864</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="n">
-        <v>18097.9692857143</v>
+        <v>9619.32857142857</v>
       </c>
       <c r="G7" t="n">
-        <v>2641234.08214286</v>
+        <v>1687826.05714286</v>
       </c>
       <c r="H7" t="n">
-        <v>0.74237015316871</v>
+        <v>1.31788523629769</v>
       </c>
       <c r="I7"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44818</v>
+        <v>44953</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="n">
-        <v>52.7801968701343</v>
+        <v>5.13894891976541</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0490018181170012</v>
+        <v>0.0176083819768147</v>
       </c>
       <c r="E8" t="n">
-        <v>0.346783836740215</v>
+        <v>-0.0509851313580177</v>
       </c>
       <c r="F8" t="n">
-        <v>7578.6</v>
+        <v>19459.2321428571</v>
       </c>
       <c r="G8" t="n">
-        <v>3433442.4</v>
+        <v>27627797.0464286</v>
       </c>
       <c r="H8" t="n">
-        <v>1.72247100580547</v>
-      </c>
-      <c r="I8" t="n">
-        <v>-0.459941152770569</v>
+        <v>0.710874300897029</v>
+      </c>
+      <c r="I8" t="e">
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45279</v>
+        <v>44998</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="n">
-        <v>409.296138546743</v>
+        <v>33.1790704053949</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0895346799829791</v>
+        <v>0.0942639400766061</v>
       </c>
       <c r="E9" t="n">
-        <v>0.386132065900496</v>
+        <v>0.0410550448373626</v>
       </c>
       <c r="F9" t="n">
-        <v>1954.575</v>
+        <v>18083.6892857143</v>
       </c>
       <c r="G9" t="n">
-        <v>458437.725</v>
+        <v>4604184.19285714</v>
       </c>
       <c r="H9" t="n">
-        <v>2.61203764736759</v>
+        <v>1.52086421401315</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.413264131384523</v>
+        <v>-1.38663346922879</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>45140</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="n">
+        <v>657.928746316773</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.624858780565361</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.489625120007815</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1823.90571428572</v>
+      </c>
+      <c r="G10" t="n">
+        <v>-61297.0821428564</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2.81817886206828</v>
+      </c>
+      <c r="I10" t="n">
+        <v>-0.310136308997868</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>45197</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="n">
+        <v>133.328381136318</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.0966021881464723</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.190986898896875</v>
+      </c>
+      <c r="F11" t="n">
+        <v>750.027857142865</v>
+      </c>
+      <c r="G11" t="n">
+        <v>273295.885714292</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2.12492260596996</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-0.718996422971846</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>45231</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="n">
+        <v>17.3551452799212</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0456410932698102</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0829762877707573</v>
+      </c>
+      <c r="F12" t="n">
+        <v>2880.99</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1527569.85</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1.23942825350176</v>
+      </c>
+      <c r="I12" t="n">
+        <v>-1.08104599872781</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>45296</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="n">
+        <v>236.595392304735</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.229962718506469</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.287726779544469</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2535.975</v>
+      </c>
+      <c r="G13" t="n">
+        <v>628582.649999999</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2.37400628248923</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-0.541019715213791</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>45331</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14" t="n">
+        <v>0.186952867332309</v>
+      </c>
+      <c r="F14" t="n">
+        <v>47179.08</v>
+      </c>
+      <c r="G14" t="n">
+        <v>17329386.9</v>
+      </c>
+      <c r="H14"/>
+      <c r="I14" t="n">
+        <v>-0.728267869600161</v>
       </c>
     </row>
   </sheetData>
@@ -2789,25 +3199,25 @@
         <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>110.528991754537</v>
+        <v>79.9725579879591</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0578152666505854</v>
+        <v>0.0836415522456026</v>
       </c>
       <c r="E2" t="n">
-        <v>0.334368448888413</v>
+        <v>0.175235931608227</v>
       </c>
       <c r="F2" t="n">
-        <v>2261.85</v>
+        <v>2500.85785714285</v>
       </c>
       <c r="G2" t="n">
-        <v>1490548.95</v>
+        <v>774402.396428567</v>
       </c>
       <c r="H2" t="n">
-        <v>2.04347620840636</v>
+        <v>1.90294098750518</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.475774709463059</v>
+        <v>-0.756376838240995</v>
       </c>
     </row>
     <row r="3">
@@ -2818,25 +3228,25 @@
         <v>16</v>
       </c>
       <c r="C3" t="n">
-        <v>145.543610583516</v>
+        <v>97.517092917943</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0876716470388422</v>
+        <v>0.0844166976160872</v>
       </c>
       <c r="E3" t="n">
-        <v>0.432978589290512</v>
+        <v>0.428172659072591</v>
       </c>
       <c r="F3" t="n">
-        <v>4122.47571428571</v>
+        <v>12305.535</v>
       </c>
       <c r="G3" t="n">
-        <v>1650464.00357143</v>
+        <v>5685082.2</v>
       </c>
       <c r="H3" t="n">
-        <v>2.16299314451045</v>
+        <v>1.9890807460505</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.363533578895795</v>
+        <v>-0.368381067992078</v>
       </c>
     </row>
     <row r="4">
@@ -2847,25 +3257,25 @@
         <v>16</v>
       </c>
       <c r="C4" t="n">
-        <v>19.0713037906123</v>
+        <v>14.3008118570891</v>
       </c>
       <c r="D4" t="n">
-        <v>0.111120888231963</v>
+        <v>0.10472695502504</v>
       </c>
       <c r="E4" t="n">
-        <v>0.23773763726534</v>
+        <v>0.226952277503813</v>
       </c>
       <c r="F4" t="n">
-        <v>7865.22</v>
+        <v>13985.22</v>
       </c>
       <c r="G4" t="n">
-        <v>1033398.975</v>
+        <v>1949681.55</v>
       </c>
       <c r="H4" t="n">
-        <v>1.28038038416888</v>
+        <v>1.15536069306266</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.623902057806076</v>
+        <v>-0.64406545468198</v>
       </c>
     </row>
     <row r="5">
@@ -2876,25 +3286,25 @@
         <v>16</v>
       </c>
       <c r="C5" t="n">
-        <v>16.9350140609002</v>
+        <v>19.273719443755</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0463166323010258</v>
+        <v>0.0768117708525735</v>
       </c>
       <c r="E5" t="n">
-        <v>0.21568387517109</v>
+        <v>0.258582477591671</v>
       </c>
       <c r="F5" t="n">
-        <v>11809.8514285714</v>
+        <v>10376.8242857143</v>
       </c>
       <c r="G5" t="n">
-        <v>10479710.4107143</v>
+        <v>2877506.33571429</v>
       </c>
       <c r="H5" t="n">
-        <v>1.2287855615693</v>
+        <v>1.28496553292348</v>
       </c>
       <c r="I5" t="n">
-        <v>-0.666182322148197</v>
+        <v>-0.587400907696447</v>
       </c>
     </row>
     <row r="6">
@@ -2905,55 +3315,51 @@
         <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>4.49444319884161</v>
+        <v>6.79493167987407</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0437964783271548</v>
+        <v>0.0279077813421051</v>
       </c>
       <c r="E6" t="n">
-        <v>0.184310511172043</v>
+        <v>0.185682797933314</v>
       </c>
       <c r="F6" t="n">
-        <v>11124.8485714286</v>
+        <v>14716.8514285714</v>
       </c>
       <c r="G6" t="n">
-        <v>2159105.4</v>
+        <v>4798781.61428571</v>
       </c>
       <c r="H6" t="n">
-        <v>0.652675896147369</v>
+        <v>0.832185094445576</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.734449896393269</v>
+        <v>-0.731228328401752</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44666</v>
+        <v>44665</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>2.89214023293876</v>
+        <v>5.52548180523963</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0252018268584692</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.153543970343754</v>
-      </c>
+        <v>0.0835954778785003</v>
+      </c>
+      <c r="E7"/>
       <c r="F7" t="n">
-        <v>17288.235</v>
+        <v>18097.9692857143</v>
       </c>
       <c r="G7" t="n">
-        <v>11318857.125</v>
+        <v>2641234.08214286</v>
       </c>
       <c r="H7" t="n">
-        <v>0.461219347030154</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-0.813767233586602</v>
-      </c>
+        <v>0.74237015316871</v>
+      </c>
+      <c r="I7"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2963,83 +3369,54 @@
         <v>16</v>
       </c>
       <c r="C8" t="n">
-        <v>105.628429740967</v>
+        <v>52.7801968701343</v>
       </c>
       <c r="D8" t="n">
-        <v>0.142353917790553</v>
+        <v>0.0490018181170012</v>
       </c>
       <c r="E8" t="n">
-        <v>0.398938311717069</v>
+        <v>0.346783836740215</v>
       </c>
       <c r="F8" t="n">
-        <v>7573.71857142857</v>
+        <v>7578.6</v>
       </c>
       <c r="G8" t="n">
-        <v>2255825.98928571</v>
+        <v>3433442.4</v>
       </c>
       <c r="H8" t="n">
-        <v>2.02378082367035</v>
+        <v>1.72247100580547</v>
       </c>
       <c r="I8" t="n">
-        <v>-0.399094254569193</v>
+        <v>-0.459941152770569</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44966</v>
+        <v>45279</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>8.00184819830957</v>
+        <v>409.296138546743</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0131382698505472</v>
+        <v>0.0895346799829791</v>
       </c>
       <c r="E9" t="n">
-        <v>0.110887957954024</v>
+        <v>0.386132065900496</v>
       </c>
       <c r="F9" t="n">
-        <v>6248.55642857143</v>
+        <v>1954.575</v>
       </c>
       <c r="G9" t="n">
-        <v>6658394.97857143</v>
+        <v>458437.725</v>
       </c>
       <c r="H9" t="n">
-        <v>0.903190308194961</v>
+        <v>2.61203764736759</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.955115614158115</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>44998</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="n">
-        <v>126.543034122329</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.154867311917387</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0.338755228520558</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3951.225</v>
-      </c>
-      <c r="G10" t="n">
-        <v>714381.225</v>
-      </c>
-      <c r="H10" t="n">
-        <v>2.10223824332676</v>
-      </c>
-      <c r="I10" t="n">
-        <v>-0.470113992943802</v>
+        <v>-0.413264131384523</v>
       </c>
     </row>
   </sheetData>
@@ -3087,340 +3464,263 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>44302</v>
+        <v>44292</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="n">
-        <v>243.295049119533</v>
+        <v>110.528991754537</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.415059873828465</v>
+        <v>0.0578152666505854</v>
       </c>
       <c r="E2" t="n">
-        <v>0.190023104440148</v>
+        <v>0.334368448888413</v>
       </c>
       <c r="F2" t="n">
-        <v>2055.11785714286</v>
+        <v>2261.85</v>
       </c>
       <c r="G2" t="n">
-        <v>-165871.125</v>
+        <v>1490548.95</v>
       </c>
       <c r="H2" t="n">
-        <v>2.38613327143824</v>
+        <v>2.04347620840636</v>
       </c>
       <c r="I2" t="n">
-        <v>-0.721193591042821</v>
+        <v>-0.475774709463059</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>44386</v>
+        <v>44371</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>1444.94054069675</v>
+        <v>145.543610583516</v>
       </c>
       <c r="D3" t="n">
-        <v>0.577927133588421</v>
+        <v>0.0876716470388422</v>
       </c>
       <c r="E3" t="n">
-        <v>0.835018144430228</v>
+        <v>0.432978589290512</v>
       </c>
       <c r="F3" t="n">
-        <v>1384.14</v>
+        <v>4122.47571428571</v>
       </c>
       <c r="G3" t="n">
-        <v>76640.25</v>
+        <v>1650464.00357143</v>
       </c>
       <c r="H3" t="n">
-        <v>3.15984997624233</v>
+        <v>2.16299314451045</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.0783040874621337</v>
+        <v>-0.363533578895795</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>44589</v>
+        <v>44452</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="n">
-        <v>60.5612033684141</v>
+        <v>19.0713037906123</v>
       </c>
       <c r="D4" t="n">
-        <v>0.166262713408938</v>
+        <v>0.111120888231963</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.0718485345186965</v>
+        <v>0.23773763726534</v>
       </c>
       <c r="F4" t="n">
-        <v>4953.66642857143</v>
+        <v>7865.22</v>
       </c>
       <c r="G4" t="n">
-        <v>953414.764285715</v>
+        <v>1033398.975</v>
       </c>
       <c r="H4" t="n">
-        <v>1.78219449613319</v>
-      </c>
-      <c r="I4" t="e">
-        <v>#NUM!</v>
+        <v>1.28038038416888</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-0.623902057806076</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>44665</v>
+        <v>44517</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>156.869264340194</v>
+        <v>16.9350140609002</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0999742912566901</v>
-      </c>
-      <c r="E5"/>
+        <v>0.0463166323010258</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.21568387517109</v>
+      </c>
       <c r="F5" t="n">
-        <v>3506.10428571429</v>
+        <v>11809.8514285714</v>
       </c>
       <c r="G5" t="n">
-        <v>1052101.76785714</v>
+        <v>10479710.4107143</v>
       </c>
       <c r="H5" t="n">
-        <v>2.1955378598709</v>
-      </c>
-      <c r="I5"/>
+        <v>1.2287855615693</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-0.666182322148197</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>44733</v>
+        <v>44589</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
       <c r="C6" t="n">
-        <v>3.42172328934366</v>
+        <v>4.49444319884161</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0375554805809119</v>
+        <v>0.0437964783271548</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.14322728968482</v>
+        <v>0.184310511172043</v>
       </c>
       <c r="F6" t="n">
-        <v>29225.04</v>
+        <v>11124.8485714286</v>
       </c>
       <c r="G6" t="n">
-        <v>9727288.65000001</v>
+        <v>2159105.4</v>
       </c>
       <c r="H6" t="n">
-        <v>0.534244885751498</v>
-      </c>
-      <c r="I6" t="e">
-        <v>#NUM!</v>
+        <v>0.652675896147369</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-0.734449896393269</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>44817</v>
+        <v>44666</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="n">
-        <v>173.070979705367</v>
+        <v>2.89214023293876</v>
       </c>
       <c r="D7" t="n">
-        <v>0.426859527793496</v>
+        <v>0.0252018268584692</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0430076588941056</v>
+        <v>0.153543970343754</v>
       </c>
       <c r="F7" t="n">
-        <v>2600.08928571429</v>
+        <v>17288.235</v>
       </c>
       <c r="G7" t="n">
-        <v>200400.675000005</v>
+        <v>11318857.125</v>
       </c>
       <c r="H7" t="n">
-        <v>2.23822425210174</v>
+        <v>0.461219347030154</v>
       </c>
       <c r="I7" t="n">
-        <v>-1.36645419746087</v>
+        <v>-0.813767233586602</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>44879</v>
+        <v>44818</v>
       </c>
       <c r="B8" t="s">
         <v>17</v>
       </c>
       <c r="C8" t="n">
-        <v>16.9540200057436</v>
+        <v>105.628429740967</v>
       </c>
       <c r="D8" t="n">
-        <v>0.131401183260687</v>
+        <v>0.142353917790553</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.089021967023526</v>
+        <v>0.398938311717069</v>
       </c>
       <c r="F8" t="n">
-        <v>20644.0714285714</v>
+        <v>7573.71857142857</v>
       </c>
       <c r="G8" t="n">
-        <v>3189276.075</v>
+        <v>2255825.98928571</v>
       </c>
       <c r="H8" t="n">
-        <v>1.22927269128908</v>
-      </c>
-      <c r="I8" t="e">
-        <v>#NUM!</v>
+        <v>2.02378082367035</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-0.399094254569193</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>44953</v>
+        <v>44966</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="n">
-        <v>1.57548757401697</v>
+        <v>8.00184819830957</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0192449199286524</v>
+        <v>0.0131382698505472</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0322295008782968</v>
+        <v>0.110887957954024</v>
       </c>
       <c r="F9" t="n">
-        <v>63472.4142857143</v>
+        <v>6248.55642857143</v>
       </c>
       <c r="G9" t="n">
-        <v>64313703.7285714</v>
+        <v>6658394.97857143</v>
       </c>
       <c r="H9" t="n">
-        <v>0.197414982211926</v>
+        <v>0.903190308194961</v>
       </c>
       <c r="I9" t="n">
-        <v>-1.49174642013085</v>
+        <v>-0.955115614158115</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>44999</v>
+        <v>44998</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="n">
-        <v>17.4458643924238</v>
+        <v>126.543034122329</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0323205086994282</v>
+        <v>0.154867311917387</v>
       </c>
       <c r="E10" t="n">
-        <v>0.146809310279103</v>
+        <v>0.338755228520558</v>
       </c>
       <c r="F10" t="n">
-        <v>11464.035</v>
+        <v>3951.225</v>
       </c>
       <c r="G10" t="n">
-        <v>11705049.525</v>
+        <v>714381.225</v>
       </c>
       <c r="H10" t="n">
-        <v>1.24169249236021</v>
+        <v>2.10223824332676</v>
       </c>
       <c r="I10" t="n">
-        <v>-0.833246401677268</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>45231</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="n">
-        <v>26.617325749677</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.20143331114612</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.1019830414486</v>
-      </c>
-      <c r="F11" t="n">
-        <v>1878.47571428571</v>
-      </c>
-      <c r="G11" t="n">
-        <v>141748.307142857</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.42516441963977</v>
-      </c>
-      <c r="I11" t="n">
-        <v>-0.991472040175493</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>45296</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="n">
-        <v>160.293015632576</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.138009949764872</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.304619300450722</v>
-      </c>
-      <c r="F12" t="n">
-        <v>2495.43</v>
-      </c>
-      <c r="G12" t="n">
-        <v>524364.15</v>
-      </c>
-      <c r="H12" t="n">
-        <v>2.20491459947009</v>
-      </c>
-      <c r="I12" t="n">
-        <v>-0.51624258355513</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>45331</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13" t="n">
-        <v>0.262140092531933</v>
-      </c>
-      <c r="F13" t="n">
-        <v>3919.605</v>
-      </c>
-      <c r="G13" t="n">
-        <v>539592.75</v>
-      </c>
-      <c r="H13"/>
-      <c r="I13" t="n">
-        <v>-0.581466551606639</v>
+        <v>-0.470113992943802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>